<commit_message>
He acabdo de cambair el coódigo, le he eañadido al Boro (B) la valencia -3 y me ha surgido un problema con el conversor de R de .xlsx a .json
</commit_message>
<xml_diff>
--- a/Hojas de Calculo/elementos.xlsx
+++ b/Hojas de Calculo/elementos.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Total" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Total!$A$1:$H$45</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Total!$A$1:$H$87</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Total!$A$1:$H$87</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Total!$A$1:$H$45</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Total!$A$1:$F$45</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Total!$B$1:$H$45</definedName>
   </definedNames>
@@ -595,12 +595,12 @@
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.41"/>
@@ -1009,7 +1009,7 @@
         <v>50</v>
       </c>
       <c r="D16" s="5" t="n">
-        <v>3</v>
+        <v>-3.3</v>
       </c>
       <c r="E16" s="4" t="n">
         <v>1</v>
@@ -1779,7 +1779,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H45"/>
+  <autoFilter ref="A1:H87"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
He añadido el Boro y hEe añadido el gitignore
</commit_message>
<xml_diff>
--- a/Hojas de Calculo/elementos.xlsx
+++ b/Hojas de Calculo/elementos.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Total" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Total!$A$1:$H$87</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Total!$A$1:$H$45</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Total!$A$1:$H$45</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Total!$A$1:$H$87</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Total!$A$1:$F$45</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Total!$B$1:$H$45</definedName>
   </definedNames>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="121">
   <si>
     <t xml:space="preserve">z</t>
   </si>
@@ -179,6 +179,9 @@
   </si>
   <si>
     <t xml:space="preserve">B </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-3,3</t>
   </si>
   <si>
     <t xml:space="preserve">Grupo13</t>
@@ -595,12 +598,12 @@
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="bottomLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.41"/>
@@ -1008,8 +1011,8 @@
       <c r="C16" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="5" t="n">
-        <v>-3.3</v>
+      <c r="D16" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="E16" s="4" t="n">
         <v>1</v>
@@ -1021,7 +1024,7 @@
         <v>13</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1029,10 +1032,10 @@
         <v>13</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D17" s="5" t="n">
         <v>3</v>
@@ -1047,7 +1050,7 @@
         <v>13</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1055,10 +1058,10 @@
         <v>31</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D18" s="5" t="n">
         <v>3</v>
@@ -1073,7 +1076,7 @@
         <v>13</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1081,10 +1084,10 @@
         <v>30</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D19" s="5" t="n">
         <v>2</v>
@@ -1099,7 +1102,7 @@
         <v>12</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1107,10 +1110,10 @@
         <v>48</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D20" s="5" t="n">
         <v>2</v>
@@ -1125,7 +1128,7 @@
         <v>12</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1133,13 +1136,13 @@
         <v>80</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E21" s="4" t="n">
         <v>1</v>
@@ -1151,7 +1154,7 @@
         <v>12</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1159,13 +1162,13 @@
         <v>29</v>
       </c>
       <c r="B22" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>63</v>
       </c>
       <c r="E22" s="4" t="n">
         <v>2</v>
@@ -1177,7 +1180,7 @@
         <v>11</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1185,10 +1188,10 @@
         <v>47</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D23" s="5" t="n">
         <v>1</v>
@@ -1203,7 +1206,7 @@
         <v>11</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1211,13 +1214,13 @@
         <v>79</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E24" s="4" t="n">
         <v>1</v>
@@ -1229,7 +1232,7 @@
         <v>11</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1237,13 +1240,13 @@
         <v>28</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E25" s="4" t="n">
         <v>1</v>
@@ -1255,7 +1258,7 @@
         <v>10</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1263,10 +1266,10 @@
         <v>46</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>46</v>
@@ -1281,7 +1284,7 @@
         <v>10</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1289,10 +1292,10 @@
         <v>78</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D27" s="0" t="s">
         <v>46</v>
@@ -1307,7 +1310,7 @@
         <v>10</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1315,13 +1318,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E28" s="4" t="n">
         <v>1</v>
@@ -1333,7 +1336,7 @@
         <v>9</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1341,13 +1344,13 @@
         <v>26</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E29" s="4" t="n">
         <v>2</v>
@@ -1359,7 +1362,7 @@
         <v>8</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1367,13 +1370,13 @@
         <v>25</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E30" s="4" t="n">
         <v>2</v>
@@ -1385,7 +1388,7 @@
         <v>7</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1393,13 +1396,13 @@
         <v>24</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E31" s="4" t="n">
         <v>2</v>
@@ -1411,7 +1414,7 @@
         <v>6</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1419,13 +1422,13 @@
         <v>22</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E32" s="4" t="n">
         <v>1</v>
@@ -1437,7 +1440,7 @@
         <v>4</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1445,10 +1448,10 @@
         <v>4</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D33" s="5" t="n">
         <v>2</v>
@@ -1463,7 +1466,7 @@
         <v>2</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1471,25 +1474,25 @@
         <v>12</v>
       </c>
       <c r="B34" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D34" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E34" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H34" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D34" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E34" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="F34" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="G34" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1497,10 +1500,10 @@
         <v>20</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D35" s="5" t="n">
         <v>2</v>
@@ -1515,7 +1518,7 @@
         <v>2</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1523,10 +1526,10 @@
         <v>38</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D36" s="5" t="n">
         <v>2</v>
@@ -1541,7 +1544,7 @@
         <v>2</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1549,10 +1552,10 @@
         <v>56</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D37" s="5" t="n">
         <v>2</v>
@@ -1567,7 +1570,7 @@
         <v>2</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1575,10 +1578,10 @@
         <v>88</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D38" s="5" t="n">
         <v>2</v>
@@ -1593,7 +1596,7 @@
         <v>2</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1601,13 +1604,13 @@
         <v>1</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E39" s="4" t="n">
         <v>28</v>
@@ -1619,7 +1622,7 @@
         <v>1</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1627,25 +1630,25 @@
         <v>3</v>
       </c>
       <c r="B40" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D40" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E40" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G40" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H40" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D40" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E40" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="F40" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="G40" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1653,10 +1656,10 @@
         <v>11</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D41" s="5" t="n">
         <v>1</v>
@@ -1671,7 +1674,7 @@
         <v>1</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1679,10 +1682,10 @@
         <v>19</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D42" s="5" t="n">
         <v>1</v>
@@ -1697,7 +1700,7 @@
         <v>1</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1705,10 +1708,10 @@
         <v>37</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D43" s="5" t="n">
         <v>1</v>
@@ -1723,7 +1726,7 @@
         <v>1</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1731,10 +1734,10 @@
         <v>55</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D44" s="5" t="n">
         <v>1</v>
@@ -1749,7 +1752,7 @@
         <v>1</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1757,10 +1760,10 @@
         <v>87</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D45" s="5" t="n">
         <v>1</v>
@@ -1775,11 +1778,11 @@
         <v>1</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H87"/>
+  <autoFilter ref="A1:H45"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
He cambiado las puntuaciones de los diferentes elementos
</commit_message>
<xml_diff>
--- a/Hojas de Calculo/elementos.xlsx
+++ b/Hojas de Calculo/elementos.xlsx
@@ -9,15 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Total" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Total!$A$1:$K$87</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="0">Total!$A$1:$I$45</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="0">Total!$B$1:$K$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Total!$A$1:$N$87</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="0">Total!$A$1:$K$45</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="0">Total!$B$1:$N$45</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="127">
   <si>
     <t>z</t>
   </si>
@@ -397,10 +397,19 @@
     <t>Longitud</t>
   </si>
   <si>
-    <t xml:space="preserve">+ valencia max. </t>
-  </si>
-  <si>
-    <t>Repeticiones</t>
+    <t xml:space="preserve">+ valencia mín </t>
+  </si>
+  <si>
+    <t>Lonjitud Puntos</t>
+  </si>
+  <si>
+    <t>Repeticiones Puntos</t>
+  </si>
+  <si>
+    <t>Valencia + Menor P</t>
+  </si>
+  <si>
+    <t>Puntos redondeados</t>
   </si>
 </sst>
 </file>
@@ -821,11 +830,13 @@
   <sheetPr>
     <tabColor rgb="FFF10D0C"/>
   </sheetPr>
-  <dimension ref="A1:K45"/>
+  <dimension ref="A1:N45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -835,11 +846,14 @@
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1"/>
+    <col min="8" max="8" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75">
+    <row r="1" spans="1:14" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -858,496 +872,745 @@
       <c r="F1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:14">
       <c r="A2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2">
-        <v>-1</v>
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
       </c>
       <c r="E2" s="4">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="F2" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D2,"-",""),",",""))</f>
-        <v>1</v>
-      </c>
-      <c r="H2" s="4">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <f>ROUNDUP(1/F2 * 10,0)</f>
+        <v>5</v>
+      </c>
+      <c r="H2" t="str">
+        <f>IF(LEN(D2)&lt;3,RIGHT(D2),IF(LEFT(D2)="-",MID(D2,2,1),LEFT(D2)))</f>
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <f>ROUNDUP(1/(-H2 + 5) * 10,0)</f>
+        <v>3</v>
+      </c>
+      <c r="J2" s="4">
         <f>ROUNDUP(1/E2 * 10,0)</f>
-        <v>5</v>
-      </c>
-      <c r="J2">
-        <v>17</v>
-      </c>
-      <c r="K2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <f>MROUND(K2,10)</f>
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>16</v>
+      </c>
+      <c r="N2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>12</v>
+        <v>106</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>107</v>
       </c>
       <c r="E3" s="4">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="F3" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D3,"-",""),",",""))</f>
-        <v>5</v>
-      </c>
-      <c r="H3" s="4">
-        <f t="shared" ref="H3:H45" si="0">ROUNDUP(1/E3 * 10,0)</f>
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <f>ROUNDUP(1/F3 * 10,0)</f>
+        <v>5</v>
+      </c>
+      <c r="H3" t="str">
+        <f>IF(LEN(D3)&lt;3,RIGHT(D3),IF(LEFT(D3)="-",MID(D3,2,1),LEFT(D3)))</f>
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>5</v>
-      </c>
-      <c r="J3">
-        <v>17</v>
-      </c>
-      <c r="K3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <f>ROUNDUP(1/(-H3 + 5) * 10,0)</f>
+        <v>3</v>
+      </c>
+      <c r="J3" s="4">
+        <f>ROUNDUP(1/E3 * 10,0)</f>
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <f>+J3+I3+G3</f>
+        <v>9</v>
+      </c>
+      <c r="L3">
+        <f>MROUND(K3,10)</f>
+        <v>10</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="E4" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D4,"-",""),",",""))</f>
-        <v>4</v>
-      </c>
-      <c r="H4" s="4">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <f>ROUNDUP(1/F4 * 10,0)</f>
+        <v>4</v>
+      </c>
+      <c r="H4" t="str">
+        <f>IF(LEN(D4)&lt;3,RIGHT(D4),IF(LEFT(D4)="-",MID(D4,2,1),LEFT(D4)))</f>
+        <v>3</v>
       </c>
       <c r="I4">
-        <v>5</v>
-      </c>
-      <c r="J4">
-        <v>17</v>
-      </c>
-      <c r="K4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <f>ROUNDUP(1/(-H4 + 5) * 10,0)</f>
+        <v>5</v>
+      </c>
+      <c r="J4" s="4">
+        <f>ROUNDUP(1/E4 * 10,0)</f>
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <f>+J4+I4+G4</f>
+        <v>12</v>
+      </c>
+      <c r="L4">
+        <f>MROUND(K4,10)</f>
+        <v>10</v>
+      </c>
+      <c r="M4">
+        <v>15</v>
+      </c>
+      <c r="N4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="E5" s="4">
         <v>3</v>
       </c>
       <c r="F5" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D5,"-",""),",",""))</f>
-        <v>5</v>
-      </c>
-      <c r="H5" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <f>ROUNDUP(1/F5 * 10,0)</f>
+        <v>4</v>
+      </c>
+      <c r="H5" t="str">
+        <f>IF(LEN(D5)&lt;3,RIGHT(D5),IF(LEFT(D5)="-",MID(D5,2,1),LEFT(D5)))</f>
+        <v>3</v>
       </c>
       <c r="I5">
-        <v>5</v>
-      </c>
-      <c r="J5">
-        <v>17</v>
-      </c>
-      <c r="K5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <f>ROUNDUP(1/(-H5 + 5) * 10,0)</f>
+        <v>5</v>
+      </c>
+      <c r="J5" s="4">
+        <f>ROUNDUP(1/E5 * 10,0)</f>
+        <v>4</v>
+      </c>
+      <c r="K5">
+        <f>+J5+I5+G5</f>
+        <v>13</v>
+      </c>
+      <c r="L5">
+        <f>MROUND(K5,10)</f>
+        <v>10</v>
+      </c>
+      <c r="M5">
+        <v>15</v>
+      </c>
+      <c r="N5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E6" s="4">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="F6" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D6,"-",""),",",""))</f>
-        <v>2</v>
-      </c>
-      <c r="H6" s="4">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <f>ROUNDUP(1/F6 * 10,0)</f>
+        <v>3</v>
+      </c>
+      <c r="H6" t="str">
+        <f>IF(LEN(D6)&lt;3,RIGHT(D6),IF(LEFT(D6)="-",MID(D6,2,1),LEFT(D6)))</f>
+        <v>2</v>
       </c>
       <c r="I6">
-        <v>10</v>
-      </c>
-      <c r="J6">
+        <f>ROUNDUP(1/(-H6 + 5) * 10,0)</f>
+        <v>4</v>
+      </c>
+      <c r="J6" s="4">
+        <f>ROUNDUP(1/E6 * 10,0)</f>
+        <v>2</v>
+      </c>
+      <c r="K6">
+        <f>+J6+I6+G6</f>
+        <v>9</v>
+      </c>
+      <c r="L6">
+        <f>MROUND(K6,10)</f>
+        <v>10</v>
+      </c>
+      <c r="M6">
         <v>16</v>
       </c>
-      <c r="K6" t="s">
+      <c r="N6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:14">
       <c r="A7">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="E7" s="4">
         <v>5</v>
       </c>
       <c r="F7" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D7,"-",""),",",""))</f>
-        <v>4</v>
-      </c>
-      <c r="H7" s="4">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <f>ROUNDUP(1/F7 * 10,0)</f>
+        <v>2</v>
+      </c>
+      <c r="H7" t="str">
+        <f>IF(LEN(D7)&lt;3,RIGHT(D7),IF(LEFT(D7)="-",MID(D7,2,1),LEFT(D7)))</f>
+        <v>1</v>
       </c>
       <c r="I7">
-        <v>5</v>
-      </c>
-      <c r="J7">
-        <v>16</v>
-      </c>
-      <c r="K7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <f>ROUNDUP(1/(-H7 + 5) * 10,0)</f>
+        <v>3</v>
+      </c>
+      <c r="J7" s="4">
+        <f>ROUNDUP(1/E7 * 10,0)</f>
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <f>+J7+I7+G7</f>
+        <v>7</v>
+      </c>
+      <c r="L7">
+        <f>MROUND(K7,10)</f>
+        <v>10</v>
+      </c>
+      <c r="M7">
+        <v>17</v>
+      </c>
+      <c r="N7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>27</v>
+        <v>87</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>88</v>
       </c>
       <c r="E8" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D8,"-",""),",",""))</f>
-        <v>4</v>
-      </c>
-      <c r="H8" s="4">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <f>ROUNDUP(1/F8 * 10,0)</f>
+        <v>4</v>
+      </c>
+      <c r="H8" t="str">
+        <f>IF(LEN(D8)&lt;3,RIGHT(D8),IF(LEFT(D8)="-",MID(D8,2,1),LEFT(D8)))</f>
+        <v>2</v>
       </c>
       <c r="I8">
-        <v>5</v>
-      </c>
-      <c r="J8">
-        <v>16</v>
-      </c>
-      <c r="K8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <f>ROUNDUP(1/(-H8 + 5) * 10,0)</f>
+        <v>4</v>
+      </c>
+      <c r="J8" s="4">
+        <f>ROUNDUP(1/E8 * 10,0)</f>
+        <v>5</v>
+      </c>
+      <c r="K8">
+        <f>+J8+I8+G8</f>
+        <v>13</v>
+      </c>
+      <c r="L8">
+        <f>MROUND(K8,10)</f>
+        <v>10</v>
+      </c>
+      <c r="M8">
+        <v>6</v>
+      </c>
+      <c r="N8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>83</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="E9" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F9" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D9,"-",""),",",""))</f>
-        <v>3</v>
-      </c>
-      <c r="H9" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="G9">
+        <f>ROUNDUP(1/F9 * 10,0)</f>
+        <v>2</v>
+      </c>
+      <c r="H9" t="str">
+        <f>IF(LEN(D9)&lt;3,RIGHT(D9),IF(LEFT(D9)="-",MID(D9,2,1),LEFT(D9)))</f>
+        <v>2</v>
       </c>
       <c r="I9">
-        <v>5</v>
-      </c>
-      <c r="J9">
-        <v>15</v>
-      </c>
-      <c r="K9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+        <f>ROUNDUP(1/(-H9 + 5) * 10,0)</f>
+        <v>4</v>
+      </c>
+      <c r="J9" s="4">
+        <f>ROUNDUP(1/E9 * 10,0)</f>
+        <v>5</v>
+      </c>
+      <c r="K9">
+        <f>+J9+I9+G9</f>
+        <v>11</v>
+      </c>
+      <c r="L9">
+        <f>MROUND(K9,10)</f>
+        <v>10</v>
+      </c>
+      <c r="M9">
+        <v>7</v>
+      </c>
+      <c r="N9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>81</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" t="s">
-        <v>31</v>
+        <v>82</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>74</v>
       </c>
       <c r="E10" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D10,"-",""),",",""))</f>
-        <v>3</v>
-      </c>
-      <c r="H10" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <f>ROUNDUP(1/F10 * 10,0)</f>
+        <v>5</v>
+      </c>
+      <c r="H10" t="str">
+        <f>IF(LEN(D10)&lt;3,RIGHT(D10),IF(LEFT(D10)="-",MID(D10,2,1),LEFT(D10)))</f>
+        <v>2</v>
       </c>
       <c r="I10">
-        <v>5</v>
-      </c>
-      <c r="J10">
-        <v>15</v>
-      </c>
-      <c r="K10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+        <f>ROUNDUP(1/(-H10 + 5) * 10,0)</f>
+        <v>4</v>
+      </c>
+      <c r="J10" s="4">
+        <f>ROUNDUP(1/E10 * 10,0)</f>
+        <v>5</v>
+      </c>
+      <c r="K10">
+        <f>+J10+I10+G10</f>
+        <v>14</v>
+      </c>
+      <c r="L10">
+        <f>MROUND(K10,10)</f>
+        <v>10</v>
+      </c>
+      <c r="M10">
+        <v>8</v>
+      </c>
+      <c r="N10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" t="s">
-        <v>31</v>
+        <v>66</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="E11" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F11" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D11,"-",""),",",""))</f>
-        <v>3</v>
-      </c>
-      <c r="H11" s="4">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <f>ROUNDUP(1/F11 * 10,0)</f>
+        <v>5</v>
+      </c>
+      <c r="H11" t="str">
+        <f>IF(LEN(D11)&lt;3,RIGHT(D11),IF(LEFT(D11)="-",MID(D11,2,1),LEFT(D11)))</f>
+        <v>1</v>
       </c>
       <c r="I11">
-        <v>5</v>
-      </c>
-      <c r="J11">
+        <f>ROUNDUP(1/(-H11 + 5) * 10,0)</f>
+        <v>3</v>
+      </c>
+      <c r="J11" s="4">
+        <f>ROUNDUP(1/E11 * 10,0)</f>
+        <v>5</v>
+      </c>
+      <c r="K11">
+        <f>+J11+I11+G11</f>
+        <v>13</v>
+      </c>
+      <c r="L11">
+        <f>MROUND(K11,10)</f>
+        <v>10</v>
+      </c>
+      <c r="M11">
+        <v>11</v>
+      </c>
+      <c r="N11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12">
-        <v>6</v>
-      </c>
-      <c r="B12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="E12" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F12" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D12,"-",""),",",""))</f>
-        <v>3</v>
-      </c>
-      <c r="H12" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <v>4</v>
+      </c>
+      <c r="G12">
+        <f>ROUNDUP(1/F12 * 10,0)</f>
+        <v>3</v>
+      </c>
+      <c r="H12" t="str">
+        <f>IF(LEN(D12)&lt;3,RIGHT(D12),IF(LEFT(D12)="-",MID(D12,2,1),LEFT(D12)))</f>
+        <v>1</v>
       </c>
       <c r="I12">
-        <v>5</v>
-      </c>
-      <c r="J12">
-        <v>14</v>
-      </c>
-      <c r="K12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+        <f>ROUNDUP(1/(-H12 + 5) * 10,0)</f>
+        <v>3</v>
+      </c>
+      <c r="J12" s="4">
+        <f>ROUNDUP(1/E12 * 10,0)</f>
+        <v>2</v>
+      </c>
+      <c r="K12">
+        <f>+J12+I12+G12</f>
+        <v>8</v>
+      </c>
+      <c r="L12">
+        <f>MROUND(K12,10)</f>
+        <v>10</v>
+      </c>
+      <c r="M12">
+        <v>17</v>
+      </c>
+      <c r="N12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="E13" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F13" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D13,"-",""),",",""))</f>
-        <v>2</v>
-      </c>
-      <c r="H13" s="4">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <v>5</v>
+      </c>
+      <c r="G13">
+        <f>ROUNDUP(1/F13 * 10,0)</f>
+        <v>2</v>
+      </c>
+      <c r="H13" t="str">
+        <f>IF(LEN(D13)&lt;3,RIGHT(D13),IF(LEFT(D13)="-",MID(D13,2,1),LEFT(D13)))</f>
+        <v>1</v>
       </c>
       <c r="I13">
-        <v>5</v>
-      </c>
-      <c r="J13">
-        <v>14</v>
-      </c>
-      <c r="K13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+        <f>ROUNDUP(1/(-H13 + 5) * 10,0)</f>
+        <v>3</v>
+      </c>
+      <c r="J13" s="4">
+        <f>ROUNDUP(1/E13 * 10,0)</f>
+        <v>4</v>
+      </c>
+      <c r="K13">
+        <f>+J13+I13+G13</f>
+        <v>9</v>
+      </c>
+      <c r="L13">
+        <f>MROUND(K13,10)</f>
+        <v>10</v>
+      </c>
+      <c r="M13">
+        <v>17</v>
+      </c>
+      <c r="N13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" t="s">
-        <v>46</v>
+        <v>110</v>
+      </c>
+      <c r="D14" s="5">
+        <v>1</v>
       </c>
       <c r="E14" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D14,"-",""),",",""))</f>
-        <v>2</v>
-      </c>
-      <c r="H14" s="4">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <f>ROUNDUP(1/F14 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="H14" t="str">
+        <f>IF(LEN(D14)&lt;3,RIGHT(D14),IF(LEFT(D14)="-",MID(D14,2,1),LEFT(D14)))</f>
+        <v>1</v>
       </c>
       <c r="I14">
-        <v>2</v>
-      </c>
-      <c r="J14">
-        <v>14</v>
-      </c>
-      <c r="K14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+        <f>ROUNDUP(1/(-H14 + 5) * 10,0)</f>
+        <v>3</v>
+      </c>
+      <c r="J14" s="4">
+        <f>ROUNDUP(1/E14 * 10,0)</f>
+        <v>5</v>
+      </c>
+      <c r="K14">
+        <f>+J14+I14+G14</f>
+        <v>18</v>
+      </c>
+      <c r="L14">
+        <f>MROUND(K14,10)</f>
+        <v>20</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15">
-        <v>82</v>
+        <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" t="s">
-        <v>46</v>
+        <v>93</v>
+      </c>
+      <c r="D15" s="5">
+        <v>2</v>
       </c>
       <c r="E15" s="4">
         <v>1</v>
       </c>
       <c r="F15" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D15,"-",""),",",""))</f>
-        <v>2</v>
-      </c>
-      <c r="H15" s="4">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <f>ROUNDUP(1/F15 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="H15" t="str">
+        <f>IF(LEN(D15)&lt;3,RIGHT(D15),IF(LEFT(D15)="-",MID(D15,2,1),LEFT(D15)))</f>
+        <v>2</v>
       </c>
       <c r="I15">
-        <v>2</v>
-      </c>
-      <c r="J15">
-        <v>14</v>
-      </c>
-      <c r="K15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
+        <f>ROUNDUP(1/(-H15 + 5) * 10,0)</f>
+        <v>4</v>
+      </c>
+      <c r="J15" s="4">
+        <f>ROUNDUP(1/E15 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="K15">
+        <f>+J15+I15+G15</f>
+        <v>24</v>
+      </c>
+      <c r="L15">
+        <f>MROUND(K15,10)</f>
+        <v>20</v>
+      </c>
+      <c r="M15">
+        <v>2</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16">
         <v>5</v>
       </c>
@@ -1367,270 +1630,406 @@
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D16,"-",""),",",""))</f>
         <v>2</v>
       </c>
-      <c r="H16" s="4">
-        <f t="shared" si="0"/>
-        <v>10</v>
+      <c r="G16">
+        <f>ROUNDUP(1/F16 * 10,0)</f>
+        <v>5</v>
+      </c>
+      <c r="H16" t="str">
+        <f>IF(LEN(D16)&lt;3,RIGHT(D16),IF(LEFT(D16)="-",MID(D16,2,1),LEFT(D16)))</f>
+        <v>3</v>
       </c>
       <c r="I16">
-        <v>2</v>
-      </c>
-      <c r="J16">
+        <f>ROUNDUP(1/(-H16 + 5) * 10,0)</f>
+        <v>5</v>
+      </c>
+      <c r="J16" s="4">
+        <f>ROUNDUP(1/E16 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="K16">
+        <f>+J16+I16+G16</f>
+        <v>20</v>
+      </c>
+      <c r="L16">
+        <f>MROUND(K16,10)</f>
+        <v>20</v>
+      </c>
+      <c r="M16">
         <v>13</v>
       </c>
-      <c r="K16" t="s">
+      <c r="N16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:14">
       <c r="A17">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" s="5">
-        <v>3</v>
+        <v>38</v>
+      </c>
+      <c r="D17" t="s">
+        <v>39</v>
       </c>
       <c r="E17" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F17" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D17,"-",""),",",""))</f>
-        <v>1</v>
-      </c>
-      <c r="H17" s="4">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <v>3</v>
+      </c>
+      <c r="G17">
+        <f>ROUNDUP(1/F17 * 10,0)</f>
+        <v>4</v>
+      </c>
+      <c r="H17" t="str">
+        <f>IF(LEN(D17)&lt;3,RIGHT(D17),IF(LEFT(D17)="-",MID(D17,2,1),LEFT(D17)))</f>
+        <v>4</v>
       </c>
       <c r="I17">
-        <v>2</v>
-      </c>
-      <c r="J17">
-        <v>13</v>
-      </c>
-      <c r="K17" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
+        <f>ROUNDUP(1/(-H17 + 5) * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="J17" s="4">
+        <f>ROUNDUP(1/E17 * 10,0)</f>
+        <v>4</v>
+      </c>
+      <c r="K17">
+        <f>+J17+I17+G17</f>
+        <v>18</v>
+      </c>
+      <c r="L17">
+        <f>MROUND(K17,10)</f>
+        <v>20</v>
+      </c>
+      <c r="M17">
+        <v>14</v>
+      </c>
+      <c r="N17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" s="5">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="D18">
+        <v>-1</v>
       </c>
       <c r="E18" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F18" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D18,"-",""),",",""))</f>
         <v>1</v>
       </c>
-      <c r="H18" s="4">
-        <f t="shared" si="0"/>
-        <v>10</v>
+      <c r="G18">
+        <f>ROUNDUP(1/F18 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="H18" t="str">
+        <f>IF(LEN(D18)&lt;3,RIGHT(D18),IF(LEFT(D18)="-",MID(D18,2,1),LEFT(D18)))</f>
+        <v>1</v>
       </c>
       <c r="I18">
-        <v>2</v>
-      </c>
-      <c r="J18">
-        <v>13</v>
-      </c>
-      <c r="K18" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
+        <f>ROUNDUP(1/(-H18 + 5) * 10,0)</f>
+        <v>3</v>
+      </c>
+      <c r="J18" s="4">
+        <f>ROUNDUP(1/E18 * 10,0)</f>
+        <v>5</v>
+      </c>
+      <c r="K18">
+        <f>+J18+I18+G18</f>
+        <v>18</v>
+      </c>
+      <c r="L18">
+        <f>MROUND(K18,10)</f>
+        <v>20</v>
+      </c>
+      <c r="M18">
+        <v>17</v>
+      </c>
+      <c r="N18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>111</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>58</v>
+        <v>112</v>
       </c>
       <c r="D19" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E19" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F19" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D19,"-",""),",",""))</f>
         <v>1</v>
       </c>
-      <c r="H19" s="4">
-        <f t="shared" si="0"/>
-        <v>10</v>
+      <c r="G19">
+        <f>ROUNDUP(1/F19 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="H19" t="str">
+        <f>IF(LEN(D19)&lt;3,RIGHT(D19),IF(LEFT(D19)="-",MID(D19,2,1),LEFT(D19)))</f>
+        <v>1</v>
       </c>
       <c r="I19">
-        <v>2</v>
-      </c>
-      <c r="J19">
+        <f>ROUNDUP(1/(-H19 + 5) * 10,0)</f>
+        <v>3</v>
+      </c>
+      <c r="J19" s="4">
+        <f>ROUNDUP(1/E19 * 10,0)</f>
+        <v>4</v>
+      </c>
+      <c r="K19">
+        <f>+J19+I19+G19</f>
+        <v>17</v>
+      </c>
+      <c r="L19">
+        <f>MROUND(K19,10)</f>
+        <v>20</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20">
         <v>12</v>
       </c>
-      <c r="K19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="A20">
-        <v>48</v>
-      </c>
       <c r="B20" t="s">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="D20" s="5">
         <v>2</v>
       </c>
       <c r="E20" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F20" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D20,"-",""),",",""))</f>
         <v>1</v>
       </c>
-      <c r="H20" s="4">
-        <f t="shared" si="0"/>
-        <v>10</v>
+      <c r="G20">
+        <f>ROUNDUP(1/F20 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="H20" t="str">
+        <f>IF(LEN(D20)&lt;3,RIGHT(D20),IF(LEFT(D20)="-",MID(D20,2,1),LEFT(D20)))</f>
+        <v>2</v>
       </c>
       <c r="I20">
-        <v>2</v>
-      </c>
-      <c r="J20">
-        <v>12</v>
-      </c>
-      <c r="K20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
+        <f>ROUNDUP(1/(-H20 + 5) * 10,0)</f>
+        <v>4</v>
+      </c>
+      <c r="J20" s="4">
+        <f>ROUNDUP(1/E20 * 10,0)</f>
+        <v>5</v>
+      </c>
+      <c r="K20">
+        <f>+J20+I20+G20</f>
+        <v>19</v>
+      </c>
+      <c r="L20">
+        <f>MROUND(K20,10)</f>
+        <v>20</v>
+      </c>
+      <c r="M20">
+        <v>2</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21">
-        <v>80</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>62</v>
+        <v>113</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>64</v>
+        <v>114</v>
+      </c>
+      <c r="D21" s="5">
+        <v>1</v>
       </c>
       <c r="E21" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F21" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D21,"-",""),",",""))</f>
-        <v>2</v>
-      </c>
-      <c r="H21" s="4">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <f>ROUNDUP(1/F21 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="H21" t="str">
+        <f>IF(LEN(D21)&lt;3,RIGHT(D21),IF(LEFT(D21)="-",MID(D21,2,1),LEFT(D21)))</f>
+        <v>1</v>
       </c>
       <c r="I21">
-        <v>2</v>
-      </c>
-      <c r="J21">
-        <v>12</v>
-      </c>
-      <c r="K21" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
+        <f>ROUNDUP(1/(-H21 + 5) * 10,0)</f>
+        <v>3</v>
+      </c>
+      <c r="J21" s="4">
+        <f>ROUNDUP(1/E21 * 10,0)</f>
+        <v>5</v>
+      </c>
+      <c r="K21">
+        <f>+J21+I21+G21</f>
+        <v>18</v>
+      </c>
+      <c r="L21">
+        <f>MROUND(K21,10)</f>
+        <v>20</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>64</v>
+        <v>98</v>
+      </c>
+      <c r="D22" s="5">
+        <v>2</v>
       </c>
       <c r="E22" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F22" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D22,"-",""),",",""))</f>
-        <v>2</v>
-      </c>
-      <c r="H22" s="4">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <f>ROUNDUP(1/F22 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="H22" t="str">
+        <f>IF(LEN(D22)&lt;3,RIGHT(D22),IF(LEFT(D22)="-",MID(D22,2,1),LEFT(D22)))</f>
+        <v>2</v>
       </c>
       <c r="I22">
-        <v>2</v>
-      </c>
-      <c r="J22">
-        <v>11</v>
-      </c>
-      <c r="K22" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
+        <f>ROUNDUP(1/(-H22 + 5) * 10,0)</f>
+        <v>4</v>
+      </c>
+      <c r="J22" s="4">
+        <f>ROUNDUP(1/E22 * 10,0)</f>
+        <v>4</v>
+      </c>
+      <c r="K22">
+        <f>+J22+I22+G22</f>
+        <v>18</v>
+      </c>
+      <c r="L22">
+        <f>MROUND(K22,10)</f>
+        <v>20</v>
+      </c>
+      <c r="M22">
+        <v>2</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" s="5">
-        <v>1</v>
+        <v>90</v>
+      </c>
+      <c r="D23" t="s">
+        <v>91</v>
       </c>
       <c r="E23" s="4">
         <v>1</v>
       </c>
       <c r="F23" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D23,"-",""),",",""))</f>
-        <v>1</v>
-      </c>
-      <c r="H23" s="4">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <v>3</v>
+      </c>
+      <c r="G23">
+        <f>ROUNDUP(1/F23 * 10,0)</f>
+        <v>4</v>
+      </c>
+      <c r="H23" t="str">
+        <f>IF(LEN(D23)&lt;3,RIGHT(D23),IF(LEFT(D23)="-",MID(D23,2,1),LEFT(D23)))</f>
+        <v>2</v>
       </c>
       <c r="I23">
-        <v>2</v>
-      </c>
-      <c r="J23">
-        <v>11</v>
-      </c>
-      <c r="K23" t="s">
+        <f>ROUNDUP(1/(-H23 + 5) * 10,0)</f>
+        <v>4</v>
+      </c>
+      <c r="J23" s="4">
+        <f>ROUNDUP(1/E23 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="K23">
+        <f>+J23+I23+G23</f>
+        <v>18</v>
+      </c>
+      <c r="L23">
+        <f>MROUND(K23,10)</f>
+        <v>20</v>
+      </c>
+      <c r="M23">
+        <v>4</v>
+      </c>
+      <c r="N23" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:14">
       <c r="A24">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
         <v>79</v>
       </c>
-      <c r="B24" t="s">
-        <v>69</v>
-      </c>
       <c r="C24" s="3" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E24" s="4">
         <v>1</v>
@@ -1639,21 +2038,38 @@
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D24,"-",""),",",""))</f>
         <v>2</v>
       </c>
-      <c r="H24" s="4">
-        <f t="shared" si="0"/>
-        <v>10</v>
+      <c r="G24">
+        <f>ROUNDUP(1/F24 * 10,0)</f>
+        <v>5</v>
+      </c>
+      <c r="H24" t="str">
+        <f>IF(LEN(D24)&lt;3,RIGHT(D24),IF(LEFT(D24)="-",MID(D24,2,1),LEFT(D24)))</f>
+        <v>2</v>
       </c>
       <c r="I24">
-        <v>2</v>
-      </c>
-      <c r="J24">
-        <v>11</v>
-      </c>
-      <c r="K24" t="s">
+        <f>ROUNDUP(1/(-H24 + 5) * 10,0)</f>
+        <v>4</v>
+      </c>
+      <c r="J24" s="4">
+        <f>ROUNDUP(1/E24 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="K24">
+        <f>+J24+I24+G24</f>
+        <v>19</v>
+      </c>
+      <c r="L24">
+        <f>MROUND(K24,10)</f>
+        <v>20</v>
+      </c>
+      <c r="M24">
+        <v>9</v>
+      </c>
+      <c r="N24" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:14">
       <c r="A25">
         <v>28</v>
       </c>
@@ -1673,267 +2089,403 @@
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D25,"-",""),",",""))</f>
         <v>2</v>
       </c>
-      <c r="H25" s="4">
-        <f t="shared" si="0"/>
-        <v>10</v>
+      <c r="G25">
+        <f>ROUNDUP(1/F25 * 10,0)</f>
+        <v>5</v>
+      </c>
+      <c r="H25" t="str">
+        <f>IF(LEN(D25)&lt;3,RIGHT(D25),IF(LEFT(D25)="-",MID(D25,2,1),LEFT(D25)))</f>
+        <v>2</v>
       </c>
       <c r="I25">
-        <v>2</v>
-      </c>
-      <c r="J25">
-        <v>10</v>
-      </c>
-      <c r="K25" t="s">
+        <f>ROUNDUP(1/(-H25 + 5) * 10,0)</f>
+        <v>4</v>
+      </c>
+      <c r="J25" s="4">
+        <f>ROUNDUP(1/E25 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="K25">
+        <f>+J25+I25+G25</f>
+        <v>19</v>
+      </c>
+      <c r="L25">
+        <f>MROUND(K25,10)</f>
+        <v>20</v>
+      </c>
+      <c r="M25">
+        <v>10</v>
+      </c>
+      <c r="N25" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:14">
       <c r="A26">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D26" t="s">
-        <v>46</v>
+        <v>58</v>
+      </c>
+      <c r="D26" s="5">
+        <v>2</v>
       </c>
       <c r="E26" s="4">
         <v>1</v>
       </c>
       <c r="F26" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D26,"-",""),",",""))</f>
-        <v>2</v>
-      </c>
-      <c r="H26" s="4">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <f>ROUNDUP(1/F26 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="H26" t="str">
+        <f>IF(LEN(D26)&lt;3,RIGHT(D26),IF(LEFT(D26)="-",MID(D26,2,1),LEFT(D26)))</f>
+        <v>2</v>
       </c>
       <c r="I26">
-        <v>2</v>
-      </c>
-      <c r="J26">
-        <v>10</v>
-      </c>
-      <c r="K26" t="s">
+        <f>ROUNDUP(1/(-H26 + 5) * 10,0)</f>
+        <v>4</v>
+      </c>
+      <c r="J26" s="4">
+        <f>ROUNDUP(1/E26 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="K26">
+        <f>+J26+I26+G26</f>
+        <v>24</v>
+      </c>
+      <c r="L26">
+        <f>MROUND(K26,10)</f>
+        <v>20</v>
+      </c>
+      <c r="M26">
+        <v>12</v>
+      </c>
+      <c r="N26" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:14">
       <c r="A27">
-        <v>78</v>
+        <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>35</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>78</v>
+        <v>36</v>
       </c>
       <c r="D27" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="E27" s="4">
         <v>1</v>
       </c>
       <c r="F27" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D27,"-",""),",",""))</f>
-        <v>2</v>
-      </c>
-      <c r="H27" s="4">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <v>3</v>
+      </c>
+      <c r="G27">
+        <f>ROUNDUP(1/F27 * 10,0)</f>
+        <v>4</v>
+      </c>
+      <c r="H27" t="str">
+        <f>IF(LEN(D27)&lt;3,RIGHT(D27),IF(LEFT(D27)="-",MID(D27,2,1),LEFT(D27)))</f>
+        <v>3</v>
       </c>
       <c r="I27">
-        <v>2</v>
-      </c>
-      <c r="J27">
-        <v>10</v>
-      </c>
-      <c r="K27" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
+        <f>ROUNDUP(1/(-H27 + 5) * 10,0)</f>
+        <v>5</v>
+      </c>
+      <c r="J27" s="4">
+        <f>ROUNDUP(1/E27 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="K27">
+        <f>+J27+I27+G27</f>
+        <v>19</v>
+      </c>
+      <c r="L27">
+        <f>MROUND(K27,10)</f>
+        <v>20</v>
+      </c>
+      <c r="M27">
+        <v>15</v>
+      </c>
+      <c r="N27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
       <c r="A28">
+        <v>34</v>
+      </c>
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B28" t="s">
-        <v>79</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>74</v>
+      <c r="D28" t="s">
+        <v>28</v>
       </c>
       <c r="E28" s="4">
         <v>1</v>
       </c>
       <c r="F28" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D28,"-",""),",",""))</f>
-        <v>2</v>
-      </c>
-      <c r="H28" s="4">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <v>4</v>
+      </c>
+      <c r="G28">
+        <f>ROUNDUP(1/F28 * 10,0)</f>
+        <v>3</v>
+      </c>
+      <c r="H28" t="str">
+        <f>IF(LEN(D28)&lt;3,RIGHT(D28),IF(LEFT(D28)="-",MID(D28,2,1),LEFT(D28)))</f>
+        <v>2</v>
       </c>
       <c r="I28">
-        <v>2</v>
-      </c>
-      <c r="J28">
-        <v>9</v>
-      </c>
-      <c r="K28" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11">
+        <f>ROUNDUP(1/(-H28 + 5) * 10,0)</f>
+        <v>4</v>
+      </c>
+      <c r="J28" s="4">
+        <f>ROUNDUP(1/E28 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="K28">
+        <f>+J28+I28+G28</f>
+        <v>17</v>
+      </c>
+      <c r="L28">
+        <f>MROUND(K28,10)</f>
+        <v>20</v>
+      </c>
+      <c r="M28">
+        <v>16</v>
+      </c>
+      <c r="N28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
       <c r="A29">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B29" t="s">
-        <v>81</v>
+        <v>115</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>74</v>
+        <v>116</v>
+      </c>
+      <c r="D29" s="5">
+        <v>1</v>
       </c>
       <c r="E29" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F29" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D29,"-",""),",",""))</f>
-        <v>2</v>
-      </c>
-      <c r="H29" s="4">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <f>ROUNDUP(1/F29 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="H29" t="str">
+        <f>IF(LEN(D29)&lt;3,RIGHT(D29),IF(LEFT(D29)="-",MID(D29,2,1),LEFT(D29)))</f>
+        <v>1</v>
       </c>
       <c r="I29">
-        <v>2</v>
-      </c>
-      <c r="J29">
-        <v>8</v>
-      </c>
-      <c r="K29" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11">
+        <f>ROUNDUP(1/(-H29 + 5) * 10,0)</f>
+        <v>3</v>
+      </c>
+      <c r="J29" s="4">
+        <f>ROUNDUP(1/E29 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="K29">
+        <f>+J29+I29+G29</f>
+        <v>23</v>
+      </c>
+      <c r="L29">
+        <f>MROUND(K29,10)</f>
+        <v>20</v>
+      </c>
+      <c r="M29">
+        <v>1</v>
+      </c>
+      <c r="N29" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
       <c r="A30">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="B30" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D30" t="s">
-        <v>85</v>
+        <v>100</v>
+      </c>
+      <c r="D30" s="5">
+        <v>2</v>
       </c>
       <c r="E30" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F30" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D30,"-",""),",",""))</f>
-        <v>5</v>
-      </c>
-      <c r="H30" s="4">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <f>ROUNDUP(1/F30 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="H30" t="str">
+        <f>IF(LEN(D30)&lt;3,RIGHT(D30),IF(LEFT(D30)="-",MID(D30,2,1),LEFT(D30)))</f>
+        <v>2</v>
       </c>
       <c r="I30">
-        <v>2</v>
-      </c>
-      <c r="J30">
-        <v>7</v>
-      </c>
-      <c r="K30" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11">
+        <f>ROUNDUP(1/(-H30 + 5) * 10,0)</f>
+        <v>4</v>
+      </c>
+      <c r="J30" s="4">
+        <f>ROUNDUP(1/E30 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="K30">
+        <f>+J30+I30+G30</f>
+        <v>24</v>
+      </c>
+      <c r="L30">
+        <f>MROUND(K30,10)</f>
+        <v>20</v>
+      </c>
+      <c r="M30">
+        <v>2</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
       <c r="A31">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="B31" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="D31" t="s">
-        <v>88</v>
+        <v>46</v>
       </c>
       <c r="E31" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F31" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D31,"-",""),",",""))</f>
-        <v>3</v>
-      </c>
-      <c r="H31" s="4">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="G31">
+        <f>ROUNDUP(1/F31 * 10,0)</f>
+        <v>5</v>
+      </c>
+      <c r="H31" t="str">
+        <f>IF(LEN(D31)&lt;3,RIGHT(D31),IF(LEFT(D31)="-",MID(D31,2,1),LEFT(D31)))</f>
+        <v>2</v>
       </c>
       <c r="I31">
-        <v>2</v>
-      </c>
-      <c r="J31">
-        <v>6</v>
-      </c>
-      <c r="K31" t="s">
+        <f>ROUNDUP(1/(-H31 + 5) * 10,0)</f>
+        <v>4</v>
+      </c>
+      <c r="J31" s="4">
+        <f>ROUNDUP(1/E31 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="K31">
+        <f>+J31+I31+G31</f>
+        <v>19</v>
+      </c>
+      <c r="L31">
+        <f>MROUND(K31,10)</f>
+        <v>20</v>
+      </c>
+      <c r="M31">
+        <v>10</v>
+      </c>
+      <c r="N31" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:14">
       <c r="A32">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="B32" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D32" t="s">
-        <v>91</v>
+        <v>68</v>
+      </c>
+      <c r="D32" s="5">
+        <v>1</v>
       </c>
       <c r="E32" s="4">
         <v>1</v>
       </c>
       <c r="F32" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D32,"-",""),",",""))</f>
-        <v>3</v>
-      </c>
-      <c r="H32" s="4">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <f>ROUNDUP(1/F32 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="H32" t="str">
+        <f>IF(LEN(D32)&lt;3,RIGHT(D32),IF(LEFT(D32)="-",MID(D32,2,1),LEFT(D32)))</f>
+        <v>1</v>
       </c>
       <c r="I32">
-        <v>2</v>
-      </c>
-      <c r="J32">
-        <v>4</v>
-      </c>
-      <c r="K32" t="s">
+        <f>ROUNDUP(1/(-H32 + 5) * 10,0)</f>
+        <v>3</v>
+      </c>
+      <c r="J32" s="4">
+        <f>ROUNDUP(1/E32 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="K32">
+        <f>+J32+I32+G32</f>
+        <v>23</v>
+      </c>
+      <c r="L32">
+        <f>MROUND(K32,10)</f>
+        <v>20</v>
+      </c>
+      <c r="M32">
+        <v>11</v>
+      </c>
+      <c r="N32" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:14">
       <c r="A33">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="B33" t="s">
-        <v>92</v>
+        <v>60</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="D33" s="5">
         <v>2</v>
@@ -1945,338 +2497,508 @@
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D33,"-",""),",",""))</f>
         <v>1</v>
       </c>
-      <c r="H33" s="4">
-        <f t="shared" si="0"/>
-        <v>10</v>
+      <c r="G33">
+        <f>ROUNDUP(1/F33 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="H33" t="str">
+        <f>IF(LEN(D33)&lt;3,RIGHT(D33),IF(LEFT(D33)="-",MID(D33,2,1),LEFT(D33)))</f>
+        <v>2</v>
       </c>
       <c r="I33">
-        <v>5</v>
-      </c>
-      <c r="J33">
-        <v>2</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11">
+        <f>ROUNDUP(1/(-H33 + 5) * 10,0)</f>
+        <v>4</v>
+      </c>
+      <c r="J33" s="4">
+        <f>ROUNDUP(1/E33 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="K33">
+        <f>+J33+I33+G33</f>
+        <v>24</v>
+      </c>
+      <c r="L33">
+        <f>MROUND(K33,10)</f>
+        <v>20</v>
+      </c>
+      <c r="M33">
+        <v>12</v>
+      </c>
+      <c r="N33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
       <c r="A34">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="B34" t="s">
-        <v>95</v>
+        <v>44</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="D34" s="5">
-        <v>2</v>
+        <v>45</v>
+      </c>
+      <c r="D34" t="s">
+        <v>46</v>
       </c>
       <c r="E34" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F34" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D34,"-",""),",",""))</f>
-        <v>1</v>
-      </c>
-      <c r="H34" s="4">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="G34">
+        <f>ROUNDUP(1/F34 * 10,0)</f>
+        <v>5</v>
+      </c>
+      <c r="H34" t="str">
+        <f>IF(LEN(D34)&lt;3,RIGHT(D34),IF(LEFT(D34)="-",MID(D34,2,1),LEFT(D34)))</f>
+        <v>2</v>
       </c>
       <c r="I34">
-        <v>5</v>
-      </c>
-      <c r="J34">
-        <v>2</v>
-      </c>
-      <c r="K34" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11">
+        <f>ROUNDUP(1/(-H34 + 5) * 10,0)</f>
+        <v>4</v>
+      </c>
+      <c r="J34" s="4">
+        <f>ROUNDUP(1/E34 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="K34">
+        <f>+J34+I34+G34</f>
+        <v>19</v>
+      </c>
+      <c r="L34">
+        <f>MROUND(K34,10)</f>
+        <v>20</v>
+      </c>
+      <c r="M34">
+        <v>14</v>
+      </c>
+      <c r="N34" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
       <c r="A35">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="B35" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="D35" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E35" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F35" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D35,"-",""),",",""))</f>
         <v>1</v>
       </c>
-      <c r="H35" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
+      <c r="G35">
+        <f>ROUNDUP(1/F35 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="H35" t="str">
+        <f>IF(LEN(D35)&lt;3,RIGHT(D35),IF(LEFT(D35)="-",MID(D35,2,1),LEFT(D35)))</f>
+        <v>1</v>
       </c>
       <c r="I35">
-        <v>5</v>
-      </c>
-      <c r="J35">
-        <v>2</v>
-      </c>
-      <c r="K35" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11">
+        <f>ROUNDUP(1/(-H35 + 5) * 10,0)</f>
+        <v>3</v>
+      </c>
+      <c r="J35" s="4">
+        <f>ROUNDUP(1/E35 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="K35">
+        <f>+J35+I35+G35</f>
+        <v>23</v>
+      </c>
+      <c r="L35">
+        <f>MROUND(K35,10)</f>
+        <v>20</v>
+      </c>
+      <c r="M35">
+        <v>1</v>
+      </c>
+      <c r="N35" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
       <c r="A36">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="B36" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D36" s="5">
         <v>2</v>
       </c>
       <c r="E36" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F36" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D36,"-",""),",",""))</f>
         <v>1</v>
       </c>
-      <c r="H36" s="4">
-        <f t="shared" si="0"/>
-        <v>10</v>
+      <c r="G36">
+        <f>ROUNDUP(1/F36 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="H36" t="str">
+        <f>IF(LEN(D36)&lt;3,RIGHT(D36),IF(LEFT(D36)="-",MID(D36,2,1),LEFT(D36)))</f>
+        <v>2</v>
       </c>
       <c r="I36">
-        <v>5</v>
-      </c>
-      <c r="J36">
-        <v>2</v>
-      </c>
-      <c r="K36" s="2" t="s">
+        <f>ROUNDUP(1/(-H36 + 5) * 10,0)</f>
+        <v>4</v>
+      </c>
+      <c r="J36" s="4">
+        <f>ROUNDUP(1/E36 * 10,0)</f>
+        <v>5</v>
+      </c>
+      <c r="K36">
+        <f>+J36+I36+G36</f>
+        <v>19</v>
+      </c>
+      <c r="L36">
+        <f>MROUND(K36,10)</f>
+        <v>20</v>
+      </c>
+      <c r="M36">
+        <v>2</v>
+      </c>
+      <c r="N36" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:14">
       <c r="A37">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="B37" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D37" s="5">
-        <v>2</v>
+        <v>78</v>
+      </c>
+      <c r="D37" t="s">
+        <v>46</v>
       </c>
       <c r="E37" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F37" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D37,"-",""),",",""))</f>
-        <v>1</v>
-      </c>
-      <c r="H37" s="4">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="G37">
+        <f>ROUNDUP(1/F37 * 10,0)</f>
+        <v>5</v>
+      </c>
+      <c r="H37" t="str">
+        <f>IF(LEN(D37)&lt;3,RIGHT(D37),IF(LEFT(D37)="-",MID(D37,2,1),LEFT(D37)))</f>
+        <v>2</v>
       </c>
       <c r="I37">
-        <v>5</v>
-      </c>
-      <c r="J37">
-        <v>2</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11">
+        <f>ROUNDUP(1/(-H37 + 5) * 10,0)</f>
+        <v>4</v>
+      </c>
+      <c r="J37" s="4">
+        <f>ROUNDUP(1/E37 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="K37">
+        <f>+J37+I37+G37</f>
+        <v>19</v>
+      </c>
+      <c r="L37">
+        <f>MROUND(K37,10)</f>
+        <v>20</v>
+      </c>
+      <c r="M37">
+        <v>10</v>
+      </c>
+      <c r="N37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
       <c r="A38">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="B38" t="s">
-        <v>103</v>
+        <v>69</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D38" s="5">
-        <v>2</v>
+        <v>70</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>71</v>
       </c>
       <c r="E38" s="4">
         <v>1</v>
       </c>
       <c r="F38" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D38,"-",""),",",""))</f>
-        <v>1</v>
-      </c>
-      <c r="H38" s="4">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <v>2</v>
+      </c>
+      <c r="G38">
+        <f>ROUNDUP(1/F38 * 10,0)</f>
+        <v>5</v>
+      </c>
+      <c r="H38" t="str">
+        <f>IF(LEN(D38)&lt;3,RIGHT(D38),IF(LEFT(D38)="-",MID(D38,2,1),LEFT(D38)))</f>
+        <v>1</v>
       </c>
       <c r="I38">
-        <v>5</v>
-      </c>
-      <c r="J38">
-        <v>2</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11">
+        <f>ROUNDUP(1/(-H38 + 5) * 10,0)</f>
+        <v>3</v>
+      </c>
+      <c r="J38" s="4">
+        <f>ROUNDUP(1/E38 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="K38">
+        <f>+J38+I38+G38</f>
+        <v>18</v>
+      </c>
+      <c r="L38">
+        <f>MROUND(K38,10)</f>
+        <v>20</v>
+      </c>
+      <c r="M38">
+        <v>11</v>
+      </c>
+      <c r="N38" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
       <c r="A39">
-        <v>1</v>
+        <v>80</v>
       </c>
       <c r="B39" t="s">
-        <v>105</v>
+        <v>62</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D39" t="s">
-        <v>107</v>
+        <v>63</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="E39" s="4">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="F39" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D39,"-",""),",",""))</f>
         <v>2</v>
       </c>
-      <c r="H39" s="4">
-        <f t="shared" si="0"/>
+      <c r="G39">
+        <f>ROUNDUP(1/F39 * 10,0)</f>
+        <v>5</v>
+      </c>
+      <c r="H39" t="str">
+        <f>IF(LEN(D39)&lt;3,RIGHT(D39),IF(LEFT(D39)="-",MID(D39,2,1),LEFT(D39)))</f>
         <v>1</v>
       </c>
       <c r="I39">
-        <v>10</v>
-      </c>
-      <c r="J39">
-        <v>1</v>
-      </c>
-      <c r="K39" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11">
+        <f>ROUNDUP(1/(-H39 + 5) * 10,0)</f>
+        <v>3</v>
+      </c>
+      <c r="J39" s="4">
+        <f>ROUNDUP(1/E39 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="K39">
+        <f>+J39+I39+G39</f>
+        <v>18</v>
+      </c>
+      <c r="L39">
+        <f>MROUND(K39,10)</f>
+        <v>20</v>
+      </c>
+      <c r="M39">
+        <v>12</v>
+      </c>
+      <c r="N39" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
       <c r="A40">
-        <v>3</v>
+        <v>82</v>
       </c>
       <c r="B40" t="s">
-        <v>109</v>
+        <v>47</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D40" s="5">
-        <v>1</v>
+        <v>48</v>
+      </c>
+      <c r="D40" t="s">
+        <v>46</v>
       </c>
       <c r="E40" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F40" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D40,"-",""),",",""))</f>
-        <v>1</v>
-      </c>
-      <c r="H40" s="4">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="G40">
+        <f>ROUNDUP(1/F40 * 10,0)</f>
+        <v>5</v>
+      </c>
+      <c r="H40" t="str">
+        <f>IF(LEN(D40)&lt;3,RIGHT(D40),IF(LEFT(D40)="-",MID(D40,2,1),LEFT(D40)))</f>
+        <v>2</v>
       </c>
       <c r="I40">
-        <v>5</v>
-      </c>
-      <c r="J40">
-        <v>1</v>
-      </c>
-      <c r="K40" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11">
+        <f>ROUNDUP(1/(-H40 + 5) * 10,0)</f>
+        <v>4</v>
+      </c>
+      <c r="J40" s="4">
+        <f>ROUNDUP(1/E40 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="K40">
+        <f>+J40+I40+G40</f>
+        <v>19</v>
+      </c>
+      <c r="L40">
+        <f>MROUND(K40,10)</f>
+        <v>20</v>
+      </c>
+      <c r="M40">
+        <v>14</v>
+      </c>
+      <c r="N40" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
       <c r="A41">
-        <v>11</v>
+        <v>87</v>
       </c>
       <c r="B41" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="D41" s="5">
         <v>1</v>
       </c>
       <c r="E41" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F41" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D41,"-",""),",",""))</f>
         <v>1</v>
       </c>
-      <c r="H41" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
+      <c r="G41">
+        <f>ROUNDUP(1/F41 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="H41" t="str">
+        <f>IF(LEN(D41)&lt;3,RIGHT(D41),IF(LEFT(D41)="-",MID(D41,2,1),LEFT(D41)))</f>
+        <v>1</v>
       </c>
       <c r="I41">
-        <v>5</v>
-      </c>
-      <c r="J41">
-        <v>1</v>
-      </c>
-      <c r="K41" s="2" t="s">
+        <f>ROUNDUP(1/(-H41 + 5) * 10,0)</f>
+        <v>3</v>
+      </c>
+      <c r="J41" s="4">
+        <f>ROUNDUP(1/E41 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="K41">
+        <f>+J41+I41+G41</f>
+        <v>23</v>
+      </c>
+      <c r="L41">
+        <f>MROUND(K41,10)</f>
+        <v>20</v>
+      </c>
+      <c r="M41">
+        <v>1</v>
+      </c>
+      <c r="N41" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:14">
       <c r="A42">
-        <v>19</v>
+        <v>88</v>
       </c>
       <c r="B42" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="D42" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E42" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F42" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D42,"-",""),",",""))</f>
         <v>1</v>
       </c>
-      <c r="H42" s="4">
-        <f t="shared" si="0"/>
-        <v>5</v>
+      <c r="G42">
+        <f>ROUNDUP(1/F42 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="H42" t="str">
+        <f>IF(LEN(D42)&lt;3,RIGHT(D42),IF(LEFT(D42)="-",MID(D42,2,1),LEFT(D42)))</f>
+        <v>2</v>
       </c>
       <c r="I42">
-        <v>5</v>
-      </c>
-      <c r="J42">
-        <v>1</v>
-      </c>
-      <c r="K42" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11">
+        <f>ROUNDUP(1/(-H42 + 5) * 10,0)</f>
+        <v>4</v>
+      </c>
+      <c r="J42" s="4">
+        <f>ROUNDUP(1/E42 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="K42">
+        <f>+J42+I42+G42</f>
+        <v>24</v>
+      </c>
+      <c r="L42">
+        <f>MROUND(K42,10)</f>
+        <v>20</v>
+      </c>
+      <c r="M42">
+        <v>2</v>
+      </c>
+      <c r="N42" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
       <c r="A43">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="B43" t="s">
-        <v>115</v>
+        <v>53</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>116</v>
+        <v>54</v>
       </c>
       <c r="D43" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E43" s="4">
         <v>1</v>
@@ -2285,66 +3007,100 @@
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D43,"-",""),",",""))</f>
         <v>1</v>
       </c>
-      <c r="H43" s="4">
-        <f t="shared" si="0"/>
-        <v>10</v>
+      <c r="G43">
+        <f>ROUNDUP(1/F43 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="H43" t="str">
+        <f>IF(LEN(D43)&lt;3,RIGHT(D43),IF(LEFT(D43)="-",MID(D43,2,1),LEFT(D43)))</f>
+        <v>3</v>
       </c>
       <c r="I43">
-        <v>5</v>
-      </c>
-      <c r="J43">
-        <v>1</v>
-      </c>
-      <c r="K43" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11">
+        <f>ROUNDUP(1/(-H43 + 5) * 10,0)</f>
+        <v>5</v>
+      </c>
+      <c r="J43" s="4">
+        <f>ROUNDUP(1/E43 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="K43">
+        <f>+J43+I43+G43</f>
+        <v>25</v>
+      </c>
+      <c r="L43">
+        <f>MROUND(K43,10)</f>
+        <v>30</v>
+      </c>
+      <c r="M43">
+        <v>13</v>
+      </c>
+      <c r="N43" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
       <c r="A44">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="B44" t="s">
-        <v>117</v>
+        <v>41</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D44" s="5">
-        <v>1</v>
+        <v>42</v>
+      </c>
+      <c r="D44" t="s">
+        <v>43</v>
       </c>
       <c r="E44" s="4">
         <v>1</v>
       </c>
       <c r="F44" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D44,"-",""),",",""))</f>
-        <v>1</v>
-      </c>
-      <c r="H44" s="4">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <v>2</v>
+      </c>
+      <c r="G44">
+        <f>ROUNDUP(1/F44 * 10,0)</f>
+        <v>5</v>
+      </c>
+      <c r="H44" t="str">
+        <f>IF(LEN(D44)&lt;3,RIGHT(D44),IF(LEFT(D44)="-",MID(D44,2,1),LEFT(D44)))</f>
+        <v>4</v>
       </c>
       <c r="I44">
-        <v>5</v>
-      </c>
-      <c r="J44">
-        <v>1</v>
-      </c>
-      <c r="K44" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11">
+        <f>ROUNDUP(1/(-H44 + 5) * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="J44" s="4">
+        <f>ROUNDUP(1/E44 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="K44">
+        <f>+J44+I44+G44</f>
+        <v>25</v>
+      </c>
+      <c r="L44">
+        <f>MROUND(K44,10)</f>
+        <v>30</v>
+      </c>
+      <c r="M44">
+        <v>14</v>
+      </c>
+      <c r="N44" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
       <c r="A45">
-        <v>87</v>
+        <v>31</v>
       </c>
       <c r="B45" t="s">
-        <v>119</v>
+        <v>55</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>120</v>
+        <v>56</v>
       </c>
       <c r="D45" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E45" s="4">
         <v>1</v>
@@ -2353,24 +3109,45 @@
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D45,"-",""),",",""))</f>
         <v>1</v>
       </c>
-      <c r="H45" s="4">
-        <f t="shared" si="0"/>
-        <v>10</v>
+      <c r="G45">
+        <f>ROUNDUP(1/F45 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="H45" t="str">
+        <f>IF(LEN(D45)&lt;3,RIGHT(D45),IF(LEFT(D45)="-",MID(D45,2,1),LEFT(D45)))</f>
+        <v>3</v>
       </c>
       <c r="I45">
-        <v>5</v>
-      </c>
-      <c r="J45">
-        <v>1</v>
-      </c>
-      <c r="K45" s="2" t="s">
-        <v>108</v>
+        <f>ROUNDUP(1/(-H45 + 5) * 10,0)</f>
+        <v>5</v>
+      </c>
+      <c r="J45" s="4">
+        <f>ROUNDUP(1/E45 * 10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="K45">
+        <f>+J45+I45+G45</f>
+        <v>25</v>
+      </c>
+      <c r="L45">
+        <f>MROUND(K45,10)</f>
+        <v>30</v>
+      </c>
+      <c r="M45">
+        <v>13</v>
+      </c>
+      <c r="N45" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K45"/>
+  <autoFilter ref="A1:N45">
+    <sortState ref="A2:N45">
+      <sortCondition ref="L1:L45"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
He cambiado las puntuaciones
</commit_message>
<xml_diff>
--- a/Hojas de Calculo/elementos.xlsx
+++ b/Hojas de Calculo/elementos.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Total" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">Total!$A$1:$N$87</definedName>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="128">
   <si>
     <t>z</t>
   </si>
@@ -400,9 +401,6 @@
     <t xml:space="preserve">+ valencia mín </t>
   </si>
   <si>
-    <t>Lonjitud Puntos</t>
-  </si>
-  <si>
     <t>Repeticiones Puntos</t>
   </si>
   <si>
@@ -410,6 +408,12 @@
   </si>
   <si>
     <t>Puntos redondeados</t>
+  </si>
+  <si>
+    <t>Longitud Puntos</t>
+  </si>
+  <si>
+    <t>1/x</t>
   </si>
 </sst>
 </file>
@@ -447,12 +451,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -467,7 +477,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -479,6 +489,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -836,7 +847,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L20" sqref="L20"/>
+      <selection pane="bottomRight" activeCell="L46" sqref="L46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -873,22 +884,22 @@
         <v>121</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>122</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>6</v>
@@ -899,406 +910,407 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
+        <v>54</v>
+      </c>
+      <c r="D2" s="5">
+        <v>3</v>
       </c>
       <c r="E2" s="4">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="F2" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D2,"-",""),",",""))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <f>ROUNDUP(1/F2 * 10,0)</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H2" t="str">
         <f>IF(LEN(D2)&lt;3,RIGHT(D2),IF(LEFT(D2)="-",MID(D2,2,1),LEFT(D2)))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I2">
-        <f>ROUNDUP(1/(-H2 + 5) * 10,0)</f>
-        <v>3</v>
+        <f>ROUNDUP(H2/4 * 10,0)</f>
+        <v>8</v>
       </c>
       <c r="J2" s="4">
         <f>ROUNDUP(1/E2 * 10,0)</f>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <f>+J2+I2+G2</f>
+        <v>28</v>
       </c>
       <c r="L2">
-        <f>MROUND(K2,10)</f>
-        <v>0</v>
+        <f>MROUND(K2,5)</f>
+        <v>30</v>
       </c>
       <c r="M2">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="N2" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>105</v>
+        <v>35</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>106</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>107</v>
+        <v>31</v>
       </c>
       <c r="E3" s="4">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="F3" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D3,"-",""),",",""))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G3">
         <f>ROUNDUP(1/F3 * 10,0)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H3" t="str">
         <f>IF(LEN(D3)&lt;3,RIGHT(D3),IF(LEFT(D3)="-",MID(D3,2,1),LEFT(D3)))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I3">
-        <f>ROUNDUP(1/(-H3 + 5) * 10,0)</f>
-        <v>3</v>
+        <f t="shared" ref="I3:I45" si="0">ROUNDUP(H3/4 * 10,0)</f>
+        <v>8</v>
       </c>
       <c r="J3" s="4">
         <f>ROUNDUP(1/E3 * 10,0)</f>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K3">
         <f>+J3+I3+G3</f>
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="L3">
-        <f>MROUND(K3,10)</f>
-        <v>10</v>
+        <f t="shared" ref="L3:L45" si="1">MROUND(K3,5)</f>
+        <v>20</v>
       </c>
       <c r="M3">
-        <v>1</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>108</v>
+        <v>15</v>
+      </c>
+      <c r="N3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E4" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F4" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D4,"-",""),",",""))</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G4">
         <f>ROUNDUP(1/F4 * 10,0)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H4" t="str">
         <f>IF(LEN(D4)&lt;3,RIGHT(D4),IF(LEFT(D4)="-",MID(D4,2,1),LEFT(D4)))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I4">
-        <f>ROUNDUP(1/(-H4 + 5) * 10,0)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="J4" s="4">
         <f>ROUNDUP(1/E4 * 10,0)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K4">
         <f>+J4+I4+G4</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="L4">
-        <f>MROUND(K4,10)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="M4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N4" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>101</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" t="s">
-        <v>31</v>
+        <v>102</v>
+      </c>
+      <c r="D5" s="5">
+        <v>2</v>
       </c>
       <c r="E5" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D5,"-",""),",",""))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G5">
         <f>ROUNDUP(1/F5 * 10,0)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="H5" t="str">
         <f>IF(LEN(D5)&lt;3,RIGHT(D5),IF(LEFT(D5)="-",MID(D5,2,1),LEFT(D5)))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I5">
-        <f>ROUNDUP(1/(-H5 + 5) * 10,0)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="J5" s="4">
         <f>ROUNDUP(1/E5 * 10,0)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K5">
         <f>+J5+I5+G5</f>
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="L5">
-        <f>MROUND(K5,10)</f>
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>20</v>
       </c>
       <c r="M5">
-        <v>15</v>
-      </c>
-      <c r="N5" t="s">
-        <v>32</v>
+        <v>2</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>92</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="s">
-        <v>25</v>
+        <v>93</v>
+      </c>
+      <c r="D6" s="5">
+        <v>2</v>
       </c>
       <c r="E6" s="4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F6" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D6,"-",""),",",""))</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G6">
         <f>ROUNDUP(1/F6 * 10,0)</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H6" t="str">
         <f>IF(LEN(D6)&lt;3,RIGHT(D6),IF(LEFT(D6)="-",MID(D6,2,1),LEFT(D6)))</f>
         <v>2</v>
       </c>
       <c r="I6">
-        <f>ROUNDUP(1/(-H6 + 5) * 10,0)</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="J6" s="4">
         <f>ROUNDUP(1/E6 * 10,0)</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="K6">
         <f>+J6+I6+G6</f>
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="L6">
-        <f>MROUND(K6,10)</f>
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>25</v>
       </c>
       <c r="M6">
-        <v>16</v>
-      </c>
-      <c r="N6" t="s">
-        <v>22</v>
+        <v>2</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
+        <v>50</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="E7" s="4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F7" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D7,"-",""),",",""))</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G7">
         <f>ROUNDUP(1/F7 * 10,0)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H7" t="str">
         <f>IF(LEN(D7)&lt;3,RIGHT(D7),IF(LEFT(D7)="-",MID(D7,2,1),LEFT(D7)))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I7">
-        <f>ROUNDUP(1/(-H7 + 5) * 10,0)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
       <c r="J7" s="4">
         <f>ROUNDUP(1/E7 * 10,0)</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="K7">
         <f>+J7+I7+G7</f>
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="L7">
-        <f>MROUND(K7,10)</f>
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>25</v>
       </c>
       <c r="M7">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="N7" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>86</v>
+        <v>14</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>87</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>88</v>
+        <v>16</v>
       </c>
       <c r="E8" s="4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F8" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D8,"-",""),",",""))</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G8">
         <f>ROUNDUP(1/F8 * 10,0)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H8" t="str">
         <f>IF(LEN(D8)&lt;3,RIGHT(D8),IF(LEFT(D8)="-",MID(D8,2,1),LEFT(D8)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I8">
-        <f>ROUNDUP(1/(-H8 + 5) * 10,0)</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="J8" s="4">
         <f>ROUNDUP(1/E8 * 10,0)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K8">
         <f>+J8+I8+G8</f>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="L8">
-        <f>MROUND(K8,10)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="M8">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="N8" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D9" t="s">
-        <v>85</v>
+        <v>61</v>
+      </c>
+      <c r="D9" s="5">
+        <v>2</v>
       </c>
       <c r="E9" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D9,"-",""),",",""))</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G9">
         <f>ROUNDUP(1/F9 * 10,0)</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H9" t="str">
         <f>IF(LEN(D9)&lt;3,RIGHT(D9),IF(LEFT(D9)="-",MID(D9,2,1),LEFT(D9)))</f>
         <v>2</v>
       </c>
       <c r="I9">
-        <f>ROUNDUP(1/(-H9 + 5) * 10,0)</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="J9" s="4">
         <f>ROUNDUP(1/E9 * 10,0)</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="K9">
         <f>+J9+I9+G9</f>
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="L9">
-        <f>MROUND(K9,10)</f>
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>25</v>
       </c>
       <c r="M9">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="N9" t="s">
         <v>59</v>
@@ -1306,290 +1318,290 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>74</v>
+        <v>98</v>
+      </c>
+      <c r="D10" s="5">
+        <v>2</v>
       </c>
       <c r="E10" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F10" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D10,"-",""),",",""))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G10">
         <f>ROUNDUP(1/F10 * 10,0)</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H10" t="str">
         <f>IF(LEN(D10)&lt;3,RIGHT(D10),IF(LEFT(D10)="-",MID(D10,2,1),LEFT(D10)))</f>
         <v>2</v>
       </c>
       <c r="I10">
-        <f>ROUNDUP(1/(-H10 + 5) * 10,0)</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="J10" s="4">
         <f>ROUNDUP(1/E10 * 10,0)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K10">
         <f>+J10+I10+G10</f>
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="L10">
-        <f>MROUND(K10,10)</f>
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>20</v>
       </c>
       <c r="M10">
-        <v>8</v>
-      </c>
-      <c r="N10" t="s">
-        <v>59</v>
+        <v>2</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>64</v>
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>39</v>
       </c>
       <c r="E11" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F11" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D11,"-",""),",",""))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G11">
         <f>ROUNDUP(1/F11 * 10,0)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H11" t="str">
         <f>IF(LEN(D11)&lt;3,RIGHT(D11),IF(LEFT(D11)="-",MID(D11,2,1),LEFT(D11)))</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I11">
-        <f>ROUNDUP(1/(-H11 + 5) * 10,0)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="J11" s="4">
         <f>ROUNDUP(1/E11 * 10,0)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K11">
         <f>+J11+I11+G11</f>
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="L11">
-        <f>MROUND(K11,10)</f>
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>20</v>
       </c>
       <c r="M11">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="N11" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>117</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" t="s">
-        <v>16</v>
+        <v>118</v>
+      </c>
+      <c r="D12" s="5">
+        <v>1</v>
       </c>
       <c r="E12" s="4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F12" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D12,"-",""),",",""))</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G12">
         <f>ROUNDUP(1/F12 * 10,0)</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H12" t="str">
         <f>IF(LEN(D12)&lt;3,RIGHT(D12),IF(LEFT(D12)="-",MID(D12,2,1),LEFT(D12)))</f>
         <v>1</v>
       </c>
       <c r="I12">
-        <f>ROUNDUP(1/(-H12 + 5) * 10,0)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="J12" s="4">
         <f>ROUNDUP(1/E12 * 10,0)</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="K12">
         <f>+J12+I12+G12</f>
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="L12">
-        <f>MROUND(K12,10)</f>
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>25</v>
       </c>
       <c r="M12">
-        <v>17</v>
-      </c>
-      <c r="N12" t="s">
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:14">
       <c r="A13">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" t="s">
-        <v>13</v>
+        <v>58</v>
+      </c>
+      <c r="D13" s="5">
+        <v>2</v>
       </c>
       <c r="E13" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F13" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D13,"-",""),",",""))</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G13">
         <f>ROUNDUP(1/F13 * 10,0)</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H13" t="str">
         <f>IF(LEN(D13)&lt;3,RIGHT(D13),IF(LEFT(D13)="-",MID(D13,2,1),LEFT(D13)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I13">
-        <f>ROUNDUP(1/(-H13 + 5) * 10,0)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="J13" s="4">
         <f>ROUNDUP(1/E13 * 10,0)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="K13">
         <f>+J13+I13+G13</f>
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="L13">
-        <f>MROUND(K13,10)</f>
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>25</v>
       </c>
       <c r="M13">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="N13" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>109</v>
+        <v>11</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D14" s="5">
-        <v>1</v>
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
       </c>
       <c r="E14" s="4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F14" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D14,"-",""),",",""))</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G14">
         <f>ROUNDUP(1/F14 * 10,0)</f>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H14" t="str">
         <f>IF(LEN(D14)&lt;3,RIGHT(D14),IF(LEFT(D14)="-",MID(D14,2,1),LEFT(D14)))</f>
         <v>1</v>
       </c>
       <c r="I14">
-        <f>ROUNDUP(1/(-H14 + 5) * 10,0)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="J14" s="4">
         <f>ROUNDUP(1/E14 * 10,0)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K14">
         <f>+J14+I14+G14</f>
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="L14">
-        <f>MROUND(K14,10)</f>
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="M14">
-        <v>1</v>
-      </c>
-      <c r="N14" s="2" t="s">
-        <v>108</v>
+        <v>17</v>
+      </c>
+      <c r="N14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:14">
       <c r="A15">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D15" s="5">
-        <v>2</v>
+        <v>80</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>74</v>
       </c>
       <c r="E15" s="4">
         <v>1</v>
       </c>
       <c r="F15" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D15,"-",""),",",""))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G15">
         <f>ROUNDUP(1/F15 * 10,0)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H15" t="str">
         <f>IF(LEN(D15)&lt;3,RIGHT(D15),IF(LEFT(D15)="-",MID(D15,2,1),LEFT(D15)))</f>
         <v>2</v>
       </c>
       <c r="I15">
-        <f>ROUNDUP(1/(-H15 + 5) * 10,0)</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="J15" s="4">
         <f>ROUNDUP(1/E15 * 10,0)</f>
@@ -1597,34 +1609,34 @@
       </c>
       <c r="K15">
         <f>+J15+I15+G15</f>
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="L15">
-        <f>MROUND(K15,10)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="M15">
-        <v>2</v>
-      </c>
-      <c r="N15" s="2" t="s">
-        <v>94</v>
+        <v>9</v>
+      </c>
+      <c r="N15" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:14">
       <c r="A16">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="E16" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F16" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D16,"-",""),",",""))</f>
@@ -1636,46 +1648,46 @@
       </c>
       <c r="H16" t="str">
         <f>IF(LEN(D16)&lt;3,RIGHT(D16),IF(LEFT(D16)="-",MID(D16,2,1),LEFT(D16)))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I16">
-        <f>ROUNDUP(1/(-H16 + 5) * 10,0)</f>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="J16" s="4">
         <f>ROUNDUP(1/E16 * 10,0)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="K16">
         <f>+J16+I16+G16</f>
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="L16">
-        <f>MROUND(K16,10)</f>
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>15</v>
       </c>
       <c r="M16">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="N16" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:14">
       <c r="A17">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>86</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>38</v>
+        <v>87</v>
       </c>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>88</v>
       </c>
       <c r="E17" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D17,"-",""),",",""))</f>
@@ -1687,97 +1699,97 @@
       </c>
       <c r="H17" t="str">
         <f>IF(LEN(D17)&lt;3,RIGHT(D17),IF(LEFT(D17)="-",MID(D17,2,1),LEFT(D17)))</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I17">
-        <f>ROUNDUP(1/(-H17 + 5) * 10,0)</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="J17" s="4">
         <f>ROUNDUP(1/E17 * 10,0)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K17">
         <f>+J17+I17+G17</f>
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="L17">
-        <f>MROUND(K17,10)</f>
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>15</v>
       </c>
       <c r="M17">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="N17" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:14">
       <c r="A18">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18">
-        <v>-1</v>
+        <v>45</v>
+      </c>
+      <c r="D18" t="s">
+        <v>46</v>
       </c>
       <c r="E18" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D18,"-",""),",",""))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G18">
         <f>ROUNDUP(1/F18 * 10,0)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H18" t="str">
         <f>IF(LEN(D18)&lt;3,RIGHT(D18),IF(LEFT(D18)="-",MID(D18,2,1),LEFT(D18)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I18">
-        <f>ROUNDUP(1/(-H18 + 5) * 10,0)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="J18" s="4">
         <f>ROUNDUP(1/E18 * 10,0)</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="K18">
         <f>+J18+I18+G18</f>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="L18">
-        <f>MROUND(K18,10)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="M18">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="N18" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:14">
       <c r="A19">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="D19" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E19" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F19" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D19,"-",""),",",""))</f>
@@ -1789,43 +1801,43 @@
       </c>
       <c r="H19" t="str">
         <f>IF(LEN(D19)&lt;3,RIGHT(D19),IF(LEFT(D19)="-",MID(D19,2,1),LEFT(D19)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I19">
-        <f>ROUNDUP(1/(-H19 + 5) * 10,0)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="J19" s="4">
         <f>ROUNDUP(1/E19 * 10,0)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="K19">
         <f>+J19+I19+G19</f>
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="L19">
-        <f>MROUND(K19,10)</f>
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>25</v>
       </c>
       <c r="M19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:14">
       <c r="A20">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="D20" s="5">
-        <v>2</v>
+        <v>9</v>
+      </c>
+      <c r="D20">
+        <v>-1</v>
       </c>
       <c r="E20" s="4">
         <v>2</v>
@@ -1840,11 +1852,11 @@
       </c>
       <c r="H20" t="str">
         <f>IF(LEN(D20)&lt;3,RIGHT(D20),IF(LEFT(D20)="-",MID(D20,2,1),LEFT(D20)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I20">
-        <f>ROUNDUP(1/(-H20 + 5) * 10,0)</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="J20" s="4">
         <f>ROUNDUP(1/E20 * 10,0)</f>
@@ -1852,85 +1864,85 @@
       </c>
       <c r="K20">
         <f>+J20+I20+G20</f>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L20">
-        <f>MROUND(K20,10)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="M20">
-        <v>2</v>
-      </c>
-      <c r="N20" s="2" t="s">
-        <v>94</v>
+        <v>17</v>
+      </c>
+      <c r="N20" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:14">
       <c r="A21">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>113</v>
+        <v>33</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D21" s="5">
-        <v>1</v>
+        <v>34</v>
+      </c>
+      <c r="D21" t="s">
+        <v>31</v>
       </c>
       <c r="E21" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F21" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D21,"-",""),",",""))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G21">
         <f>ROUNDUP(1/F21 * 10,0)</f>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="H21" t="str">
         <f>IF(LEN(D21)&lt;3,RIGHT(D21),IF(LEFT(D21)="-",MID(D21,2,1),LEFT(D21)))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I21">
-        <f>ROUNDUP(1/(-H21 + 5) * 10,0)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
       <c r="J21" s="4">
         <f>ROUNDUP(1/E21 * 10,0)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K21">
         <f>+J21+I21+G21</f>
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L21">
-        <f>MROUND(K21,10)</f>
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>15</v>
       </c>
       <c r="M21">
-        <v>1</v>
-      </c>
-      <c r="N21" s="2" t="s">
-        <v>108</v>
+        <v>15</v>
+      </c>
+      <c r="N21" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:14">
       <c r="A22">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="B22" t="s">
-        <v>97</v>
+        <v>119</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="D22" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E22" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F22" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D22,"-",""),",",""))</f>
@@ -1942,62 +1954,62 @@
       </c>
       <c r="H22" t="str">
         <f>IF(LEN(D22)&lt;3,RIGHT(D22),IF(LEFT(D22)="-",MID(D22,2,1),LEFT(D22)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I22">
-        <f>ROUNDUP(1/(-H22 + 5) * 10,0)</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="J22" s="4">
         <f>ROUNDUP(1/E22 * 10,0)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="K22">
         <f>+J22+I22+G22</f>
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="L22">
-        <f>MROUND(K22,10)</f>
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>25</v>
       </c>
       <c r="M22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:14">
       <c r="A23">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D23" t="s">
-        <v>91</v>
+        <v>56</v>
+      </c>
+      <c r="D23" s="5">
+        <v>3</v>
       </c>
       <c r="E23" s="4">
         <v>1</v>
       </c>
       <c r="F23" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D23,"-",""),",",""))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G23">
         <f>ROUNDUP(1/F23 * 10,0)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="H23" t="str">
         <f>IF(LEN(D23)&lt;3,RIGHT(D23),IF(LEFT(D23)="-",MID(D23,2,1),LEFT(D23)))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I23">
-        <f>ROUNDUP(1/(-H23 + 5) * 10,0)</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
       <c r="J23" s="4">
         <f>ROUNDUP(1/E23 * 10,0)</f>
@@ -2005,34 +2017,34 @@
       </c>
       <c r="K23">
         <f>+J23+I23+G23</f>
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="L23">
-        <f>MROUND(K23,10)</f>
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>30</v>
       </c>
       <c r="M23">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="N23" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:14">
       <c r="A24">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>74</v>
+        <v>106</v>
+      </c>
+      <c r="D24" t="s">
+        <v>107</v>
       </c>
       <c r="E24" s="4">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="F24" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D24,"-",""),",",""))</f>
@@ -2044,46 +2056,45 @@
       </c>
       <c r="H24" t="str">
         <f>IF(LEN(D24)&lt;3,RIGHT(D24),IF(LEFT(D24)="-",MID(D24,2,1),LEFT(D24)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I24">
-        <f>ROUNDUP(1/(-H24 + 5) * 10,0)</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="J24" s="4">
         <f>ROUNDUP(1/E24 * 10,0)</f>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="K24">
         <f>+J24+I24+G24</f>
-        <v>19</v>
-      </c>
-      <c r="L24">
-        <f>MROUND(K24,10)</f>
-        <v>20</v>
+        <v>9</v>
+      </c>
+      <c r="L24" s="7">
+        <v>10</v>
       </c>
       <c r="M24">
-        <v>9</v>
-      </c>
-      <c r="N24" t="s">
-        <v>59</v>
+        <v>1</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:14">
       <c r="A25">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>74</v>
       </c>
       <c r="E25" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F25" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D25,"-",""),",",""))</f>
@@ -2098,23 +2109,23 @@
         <v>2</v>
       </c>
       <c r="I25">
-        <f>ROUNDUP(1/(-H25 + 5) * 10,0)</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="J25" s="4">
         <f>ROUNDUP(1/E25 * 10,0)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="K25">
         <f>+J25+I25+G25</f>
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="L25">
-        <f>MROUND(K25,10)</f>
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>15</v>
       </c>
       <c r="M25">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="N25" t="s">
         <v>59</v>
@@ -2122,19 +2133,19 @@
     </row>
     <row r="26" spans="1:14">
       <c r="A26">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>58</v>
+        <v>110</v>
       </c>
       <c r="D26" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E26" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F26" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D26,"-",""),",",""))</f>
@@ -2146,163 +2157,163 @@
       </c>
       <c r="H26" t="str">
         <f>IF(LEN(D26)&lt;3,RIGHT(D26),IF(LEFT(D26)="-",MID(D26,2,1),LEFT(D26)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I26">
-        <f>ROUNDUP(1/(-H26 + 5) * 10,0)</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="J26" s="4">
         <f>ROUNDUP(1/E26 * 10,0)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="K26">
         <f>+J26+I26+G26</f>
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="L26">
-        <f>MROUND(K26,10)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="M26">
-        <v>12</v>
-      </c>
-      <c r="N26" t="s">
-        <v>59</v>
+        <v>1</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:14">
       <c r="A27">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>35</v>
+        <v>95</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" t="s">
-        <v>31</v>
+        <v>96</v>
+      </c>
+      <c r="D27" s="5">
+        <v>2</v>
       </c>
       <c r="E27" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F27" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D27,"-",""),",",""))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G27">
         <f>ROUNDUP(1/F27 * 10,0)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="H27" t="str">
         <f>IF(LEN(D27)&lt;3,RIGHT(D27),IF(LEFT(D27)="-",MID(D27,2,1),LEFT(D27)))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I27">
-        <f>ROUNDUP(1/(-H27 + 5) * 10,0)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="J27" s="4">
         <f>ROUNDUP(1/E27 * 10,0)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="K27">
         <f>+J27+I27+G27</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L27">
-        <f>MROUND(K27,10)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="M27">
-        <v>15</v>
-      </c>
-      <c r="N27" t="s">
-        <v>32</v>
+        <v>2</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:14">
       <c r="A28">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>83</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>27</v>
+        <v>84</v>
       </c>
       <c r="D28" t="s">
-        <v>28</v>
+        <v>85</v>
       </c>
       <c r="E28" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F28" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D28,"-",""),",",""))</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G28">
         <f>ROUNDUP(1/F28 * 10,0)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H28" t="str">
         <f>IF(LEN(D28)&lt;3,RIGHT(D28),IF(LEFT(D28)="-",MID(D28,2,1),LEFT(D28)))</f>
         <v>2</v>
       </c>
       <c r="I28">
-        <f>ROUNDUP(1/(-H28 + 5) * 10,0)</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="J28" s="4">
         <f>ROUNDUP(1/E28 * 10,0)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="K28">
         <f>+J28+I28+G28</f>
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="L28">
-        <f>MROUND(K28,10)</f>
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
       <c r="M28">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="N28" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:14">
       <c r="A29">
-        <v>37</v>
+        <v>80</v>
       </c>
       <c r="B29" t="s">
-        <v>115</v>
+        <v>62</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="D29" s="5">
-        <v>1</v>
+        <v>63</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="E29" s="4">
         <v>1</v>
       </c>
       <c r="F29" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D29,"-",""),",",""))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G29">
         <f>ROUNDUP(1/F29 * 10,0)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H29" t="str">
         <f>IF(LEN(D29)&lt;3,RIGHT(D29),IF(LEFT(D29)="-",MID(D29,2,1),LEFT(D29)))</f>
         <v>1</v>
       </c>
       <c r="I29">
-        <f>ROUNDUP(1/(-H29 + 5) * 10,0)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="J29" s="4">
@@ -2311,50 +2322,50 @@
       </c>
       <c r="K29">
         <f>+J29+I29+G29</f>
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="L29">
-        <f>MROUND(K29,10)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="M29">
-        <v>1</v>
-      </c>
-      <c r="N29" s="2" t="s">
-        <v>108</v>
+        <v>12</v>
+      </c>
+      <c r="N29" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:14">
       <c r="A30">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>99</v>
+        <v>72</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D30" s="5">
-        <v>2</v>
+        <v>73</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>74</v>
       </c>
       <c r="E30" s="4">
         <v>1</v>
       </c>
       <c r="F30" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D30,"-",""),",",""))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G30">
         <f>ROUNDUP(1/F30 * 10,0)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H30" t="str">
         <f>IF(LEN(D30)&lt;3,RIGHT(D30),IF(LEFT(D30)="-",MID(D30,2,1),LEFT(D30)))</f>
         <v>2</v>
       </c>
       <c r="I30">
-        <f>ROUNDUP(1/(-H30 + 5) * 10,0)</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="J30" s="4">
         <f>ROUNDUP(1/E30 * 10,0)</f>
@@ -2362,100 +2373,100 @@
       </c>
       <c r="K30">
         <f>+J30+I30+G30</f>
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="L30">
-        <f>MROUND(K30,10)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="M30">
-        <v>2</v>
-      </c>
-      <c r="N30" s="2" t="s">
-        <v>94</v>
+        <v>10</v>
+      </c>
+      <c r="N30" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:14">
       <c r="A31">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>75</v>
+        <v>29</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>76</v>
+        <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="E31" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F31" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D31,"-",""),",",""))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G31">
         <f>ROUNDUP(1/F31 * 10,0)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H31" t="str">
         <f>IF(LEN(D31)&lt;3,RIGHT(D31),IF(LEFT(D31)="-",MID(D31,2,1),LEFT(D31)))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I31">
-        <f>ROUNDUP(1/(-H31 + 5) * 10,0)</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
       <c r="J31" s="4">
         <f>ROUNDUP(1/E31 * 10,0)</f>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="K31">
         <f>+J31+I31+G31</f>
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="L31">
-        <f>MROUND(K31,10)</f>
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>15</v>
       </c>
       <c r="M31">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="N31" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:14">
       <c r="A32">
-        <v>47</v>
+        <v>79</v>
       </c>
       <c r="B32" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D32" s="5">
-        <v>1</v>
+        <v>70</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>71</v>
       </c>
       <c r="E32" s="4">
         <v>1</v>
       </c>
       <c r="F32" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D32,"-",""),",",""))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G32">
         <f>ROUNDUP(1/F32 * 10,0)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H32" t="str">
         <f>IF(LEN(D32)&lt;3,RIGHT(D32),IF(LEFT(D32)="-",MID(D32,2,1),LEFT(D32)))</f>
         <v>1</v>
       </c>
       <c r="I32">
-        <f>ROUNDUP(1/(-H32 + 5) * 10,0)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="J32" s="4">
@@ -2464,10 +2475,10 @@
       </c>
       <c r="K32">
         <f>+J32+I32+G32</f>
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="L32">
-        <f>MROUND(K32,10)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="M32">
@@ -2479,64 +2490,62 @@
     </row>
     <row r="33" spans="1:14">
       <c r="A33">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D33" s="5">
-        <v>2</v>
+        <v>20</v>
+      </c>
+      <c r="D33" t="s">
+        <v>21</v>
       </c>
       <c r="E33" s="4">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="F33" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D33,"-",""),",",""))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G33">
         <f>ROUNDUP(1/F33 * 10,0)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H33" t="str">
         <f>IF(LEN(D33)&lt;3,RIGHT(D33),IF(LEFT(D33)="-",MID(D33,2,1),LEFT(D33)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I33">
-        <f>ROUNDUP(1/(-H33 + 5) * 10,0)</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="J33" s="4">
         <f>ROUNDUP(1/E33 * 10,0)</f>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="K33">
-        <f>+J33+I33+G33</f>
-        <v>24</v>
-      </c>
-      <c r="L33">
-        <f>MROUND(K33,10)</f>
-        <v>20</v>
+        <v>1</v>
+      </c>
+      <c r="L33" s="7">
+        <v>5</v>
       </c>
       <c r="M33">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="N33" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:14">
       <c r="A34">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B34" t="s">
-        <v>44</v>
+        <v>75</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="D34" t="s">
         <v>46</v>
@@ -2557,8 +2566,8 @@
         <v>2</v>
       </c>
       <c r="I34">
-        <f>ROUNDUP(1/(-H34 + 5) * 10,0)</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="J34" s="4">
         <f>ROUNDUP(1/E34 * 10,0)</f>
@@ -2566,28 +2575,28 @@
       </c>
       <c r="K34">
         <f>+J34+I34+G34</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L34">
-        <f>MROUND(K34,10)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="M34">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="N34" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:14">
       <c r="A35">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B35" t="s">
-        <v>117</v>
+        <v>67</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>118</v>
+        <v>68</v>
       </c>
       <c r="D35" s="5">
         <v>1</v>
@@ -2608,7 +2617,7 @@
         <v>1</v>
       </c>
       <c r="I35">
-        <f>ROUNDUP(1/(-H35 + 5) * 10,0)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="J35" s="4">
@@ -2620,76 +2629,76 @@
         <v>23</v>
       </c>
       <c r="L35">
-        <f>MROUND(K35,10)</f>
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>25</v>
       </c>
       <c r="M35">
-        <v>1</v>
-      </c>
-      <c r="N35" s="2" t="s">
-        <v>108</v>
+        <v>11</v>
+      </c>
+      <c r="N35" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:14">
       <c r="A36">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="B36" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D36" s="5">
-        <v>2</v>
+        <v>78</v>
+      </c>
+      <c r="D36" t="s">
+        <v>46</v>
       </c>
       <c r="E36" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F36" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D36,"-",""),",",""))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G36">
         <f>ROUNDUP(1/F36 * 10,0)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H36" t="str">
         <f>IF(LEN(D36)&lt;3,RIGHT(D36),IF(LEFT(D36)="-",MID(D36,2,1),LEFT(D36)))</f>
         <v>2</v>
       </c>
       <c r="I36">
-        <f>ROUNDUP(1/(-H36 + 5) * 10,0)</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="J36" s="4">
         <f>ROUNDUP(1/E36 * 10,0)</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="K36">
         <f>+J36+I36+G36</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L36">
-        <f>MROUND(K36,10)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="M36">
-        <v>2</v>
-      </c>
-      <c r="N36" s="2" t="s">
-        <v>94</v>
+        <v>10</v>
+      </c>
+      <c r="N36" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:14">
       <c r="A37">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B37" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="D37" t="s">
         <v>46</v>
@@ -2710,8 +2719,8 @@
         <v>2</v>
       </c>
       <c r="I37">
-        <f>ROUNDUP(1/(-H37 + 5) * 10,0)</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="J37" s="4">
         <f>ROUNDUP(1/E37 * 10,0)</f>
@@ -2719,101 +2728,101 @@
       </c>
       <c r="K37">
         <f>+J37+I37+G37</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L37">
-        <f>MROUND(K37,10)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="M37">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="N37" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:14">
       <c r="A38">
-        <v>79</v>
+        <v>19</v>
       </c>
       <c r="B38" t="s">
-        <v>69</v>
+        <v>113</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>71</v>
+        <v>114</v>
+      </c>
+      <c r="D38" s="5">
+        <v>1</v>
       </c>
       <c r="E38" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F38" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D38,"-",""),",",""))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G38">
         <f>ROUNDUP(1/F38 * 10,0)</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H38" t="str">
         <f>IF(LEN(D38)&lt;3,RIGHT(D38),IF(LEFT(D38)="-",MID(D38,2,1),LEFT(D38)))</f>
         <v>1</v>
       </c>
       <c r="I38">
-        <f>ROUNDUP(1/(-H38 + 5) * 10,0)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="J38" s="4">
         <f>ROUNDUP(1/E38 * 10,0)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="K38">
         <f>+J38+I38+G38</f>
         <v>18</v>
       </c>
       <c r="L38">
-        <f>MROUND(K38,10)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="M38">
-        <v>11</v>
-      </c>
-      <c r="N38" t="s">
-        <v>59</v>
+        <v>1</v>
+      </c>
+      <c r="N38" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="39" spans="1:14">
       <c r="A39">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="B39" t="s">
-        <v>62</v>
+        <v>103</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>64</v>
+        <v>104</v>
+      </c>
+      <c r="D39" s="5">
+        <v>2</v>
       </c>
       <c r="E39" s="4">
         <v>1</v>
       </c>
       <c r="F39" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D39,"-",""),",",""))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G39">
         <f>ROUNDUP(1/F39 * 10,0)</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H39" t="str">
         <f>IF(LEN(D39)&lt;3,RIGHT(D39),IF(LEFT(D39)="-",MID(D39,2,1),LEFT(D39)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I39">
-        <f>ROUNDUP(1/(-H39 + 5) * 10,0)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="J39" s="4">
         <f>ROUNDUP(1/E39 * 10,0)</f>
@@ -2821,50 +2830,50 @@
       </c>
       <c r="K39">
         <f>+J39+I39+G39</f>
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="L39">
-        <f>MROUND(K39,10)</f>
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>25</v>
       </c>
       <c r="M39">
-        <v>12</v>
-      </c>
-      <c r="N39" t="s">
-        <v>59</v>
+        <v>2</v>
+      </c>
+      <c r="N39" s="2" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:14">
       <c r="A40">
-        <v>82</v>
+        <v>37</v>
       </c>
       <c r="B40" t="s">
-        <v>47</v>
+        <v>115</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D40" t="s">
-        <v>46</v>
+        <v>116</v>
+      </c>
+      <c r="D40" s="5">
+        <v>1</v>
       </c>
       <c r="E40" s="4">
         <v>1</v>
       </c>
       <c r="F40" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D40,"-",""),",",""))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G40">
         <f>ROUNDUP(1/F40 * 10,0)</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H40" t="str">
         <f>IF(LEN(D40)&lt;3,RIGHT(D40),IF(LEFT(D40)="-",MID(D40,2,1),LEFT(D40)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I40">
-        <f>ROUNDUP(1/(-H40 + 5) * 10,0)</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="J40" s="4">
         <f>ROUNDUP(1/E40 * 10,0)</f>
@@ -2872,50 +2881,50 @@
       </c>
       <c r="K40">
         <f>+J40+I40+G40</f>
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L40">
-        <f>MROUND(K40,10)</f>
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>25</v>
       </c>
       <c r="M40">
-        <v>14</v>
-      </c>
-      <c r="N40" t="s">
-        <v>40</v>
+        <v>1</v>
+      </c>
+      <c r="N40" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="41" spans="1:14">
       <c r="A41">
-        <v>87</v>
+        <v>34</v>
       </c>
       <c r="B41" t="s">
-        <v>119</v>
+        <v>26</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="D41" s="5">
-        <v>1</v>
+        <v>27</v>
+      </c>
+      <c r="D41" t="s">
+        <v>28</v>
       </c>
       <c r="E41" s="4">
         <v>1</v>
       </c>
       <c r="F41" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D41,"-",""),",",""))</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G41">
         <f>ROUNDUP(1/F41 * 10,0)</f>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H41" t="str">
         <f>IF(LEN(D41)&lt;3,RIGHT(D41),IF(LEFT(D41)="-",MID(D41,2,1),LEFT(D41)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I41">
-        <f>ROUNDUP(1/(-H41 + 5) * 10,0)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="J41" s="4">
         <f>ROUNDUP(1/E41 * 10,0)</f>
@@ -2923,50 +2932,50 @@
       </c>
       <c r="K41">
         <f>+J41+I41+G41</f>
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="L41">
-        <f>MROUND(K41,10)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="M41">
-        <v>1</v>
-      </c>
-      <c r="N41" s="2" t="s">
-        <v>108</v>
+        <v>16</v>
+      </c>
+      <c r="N41" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="1:14">
       <c r="A42">
-        <v>88</v>
+        <v>14</v>
       </c>
       <c r="B42" t="s">
-        <v>103</v>
+        <v>41</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D42" s="5">
-        <v>2</v>
+        <v>42</v>
+      </c>
+      <c r="D42" t="s">
+        <v>43</v>
       </c>
       <c r="E42" s="4">
         <v>1</v>
       </c>
       <c r="F42" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D42,"-",""),",",""))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G42">
         <f>ROUNDUP(1/F42 * 10,0)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H42" t="str">
         <f>IF(LEN(D42)&lt;3,RIGHT(D42),IF(LEFT(D42)="-",MID(D42,2,1),LEFT(D42)))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I42">
-        <f>ROUNDUP(1/(-H42 + 5) * 10,0)</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="J42" s="4">
         <f>ROUNDUP(1/E42 * 10,0)</f>
@@ -2974,34 +2983,34 @@
       </c>
       <c r="K42">
         <f>+J42+I42+G42</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L42">
-        <f>MROUND(K42,10)</f>
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>25</v>
       </c>
       <c r="M42">
-        <v>2</v>
-      </c>
-      <c r="N42" s="2" t="s">
-        <v>94</v>
+        <v>14</v>
+      </c>
+      <c r="N42" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:14">
       <c r="A43">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B43" t="s">
-        <v>53</v>
+        <v>111</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>54</v>
+        <v>112</v>
       </c>
       <c r="D43" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E43" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F43" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D43,"-",""),",",""))</f>
@@ -3013,62 +3022,62 @@
       </c>
       <c r="H43" t="str">
         <f>IF(LEN(D43)&lt;3,RIGHT(D43),IF(LEFT(D43)="-",MID(D43,2,1),LEFT(D43)))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I43">
-        <f>ROUNDUP(1/(-H43 + 5) * 10,0)</f>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="J43" s="4">
         <f>ROUNDUP(1/E43 * 10,0)</f>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="K43">
         <f>+J43+I43+G43</f>
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="L43">
-        <f>MROUND(K43,10)</f>
-        <v>30</v>
+        <f t="shared" si="1"/>
+        <v>15</v>
       </c>
       <c r="M43">
-        <v>13</v>
-      </c>
-      <c r="N43" t="s">
-        <v>52</v>
+        <v>1</v>
+      </c>
+      <c r="N43" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="44" spans="1:14">
       <c r="A44">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B44" t="s">
-        <v>41</v>
+        <v>89</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="D44" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="E44" s="4">
         <v>1</v>
       </c>
       <c r="F44" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D44,"-",""),",",""))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G44">
         <f>ROUNDUP(1/F44 * 10,0)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H44" t="str">
         <f>IF(LEN(D44)&lt;3,RIGHT(D44),IF(LEFT(D44)="-",MID(D44,2,1),LEFT(D44)))</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I44">
-        <f>ROUNDUP(1/(-H44 + 5) * 10,0)</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="J44" s="4">
         <f>ROUNDUP(1/E44 * 10,0)</f>
@@ -3076,74 +3085,74 @@
       </c>
       <c r="K44">
         <f>+J44+I44+G44</f>
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="L44">
-        <f>MROUND(K44,10)</f>
-        <v>30</v>
+        <f t="shared" si="1"/>
+        <v>20</v>
       </c>
       <c r="M44">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="N44" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:14">
       <c r="A45">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="B45" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D45" s="5">
-        <v>3</v>
+        <v>18</v>
+      </c>
+      <c r="D45" t="s">
+        <v>13</v>
       </c>
       <c r="E45" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F45" s="4">
         <f>+LEN(SUBSTITUTE(SUBSTITUTE(D45,"-",""),",",""))</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G45">
         <f>ROUNDUP(1/F45 * 10,0)</f>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H45" t="str">
         <f>IF(LEN(D45)&lt;3,RIGHT(D45),IF(LEFT(D45)="-",MID(D45,2,1),LEFT(D45)))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I45">
-        <f>ROUNDUP(1/(-H45 + 5) * 10,0)</f>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="J45" s="4">
         <f>ROUNDUP(1/E45 * 10,0)</f>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="K45">
         <f>+J45+I45+G45</f>
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="L45">
-        <f>MROUND(K45,10)</f>
-        <v>30</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
       <c r="M45">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="N45" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:N45">
     <sortState ref="A2:N45">
-      <sortCondition ref="L1:L45"/>
+      <sortCondition ref="B1:B45"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -3153,4 +3162,88 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>3</v>
+      </c>
+      <c r="D1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <f>-A5+5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <f t="shared" ref="B6:B8" si="0">-A6+5</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="D10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>